<commit_message>
bug fix : [instructions.md] mull operation. Rd = (Rd * Rs) & 0xFFFF -> Rd = (Rd * Rs) & 0xFFFFFFFF
</commit_message>
<xml_diff>
--- a/instructions/mist32_isa.xlsx
+++ b/instructions/mist32_isa.xlsx
@@ -586,10 +586,6 @@
   </si>
   <si>
     <t>Rd = Rd - Rs</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Rd = (Rd * Rs) &amp; 0xFFFF</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1945,6 +1941,10 @@
     <rPh sb="0" eb="4">
       <t>フゴウカクチョウ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Rd = (Rd * Rs) &amp; 0xFFFFFFFF</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2711,8 +2711,8 @@
   </sheetPr>
   <dimension ref="A2:AK1031"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A251" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E143" sqref="E143"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2751,7 +2751,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.15">
       <c r="C3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -2764,52 +2764,52 @@
     </row>
     <row r="6" spans="1:19" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
+        <v>401</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>402</v>
       </c>
-      <c r="B6" s="18" t="s">
-        <v>403</v>
-      </c>
       <c r="C6" s="18" t="s">
+        <v>371</v>
+      </c>
+      <c r="D6" s="18" t="s">
         <v>372</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="E6" s="18" t="s">
         <v>373</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="F6" s="18" t="s">
         <v>374</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="G6" s="18" t="s">
         <v>375</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="H6" s="18" t="s">
+        <v>385</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>384</v>
+      </c>
+      <c r="J6" s="18" t="s">
         <v>376</v>
       </c>
-      <c r="H6" s="18" t="s">
-        <v>386</v>
-      </c>
-      <c r="I6" s="18" t="s">
-        <v>385</v>
-      </c>
-      <c r="J6" s="18" t="s">
-        <v>377</v>
-      </c>
       <c r="K6" s="18" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L6" s="29" t="s">
+        <v>378</v>
+      </c>
+      <c r="M6" s="43" t="s">
         <v>379</v>
-      </c>
-      <c r="M6" s="43" t="s">
-        <v>380</v>
       </c>
       <c r="N6" s="26" t="s">
         <v>76</v>
       </c>
       <c r="O6" s="33" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="P6" s="33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="Q6" s="19" t="s">
         <v>41</v>
@@ -2830,7 +2830,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F7" s="15" t="s">
         <v>0</v>
@@ -2843,7 +2843,7 @@
         <v>16</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J7" s="15" t="s">
         <v>121</v>
@@ -2869,7 +2869,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>3</v>
@@ -2882,7 +2882,7 @@
         <v>16</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>122</v>
@@ -2908,7 +2908,7 @@
         <v>48</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F9" s="22" t="s">
         <v>63</v>
@@ -2921,10 +2921,10 @@
         <v>16</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>123</v>
+        <v>409</v>
       </c>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
@@ -2947,7 +2947,7 @@
         <v>49</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F10" s="22" t="s">
         <v>47</v>
@@ -2960,10 +2960,10 @@
         <v>16</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
@@ -2983,11 +2983,11 @@
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E11" s="22"/>
       <c r="F11" s="22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G11" s="6" t="str">
         <f t="shared" si="2"/>
@@ -2997,10 +2997,10 @@
         <v>16</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
@@ -3024,11 +3024,11 @@
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E12" s="22"/>
       <c r="F12" s="22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G12" s="22" t="str">
         <f t="shared" si="2"/>
@@ -3038,10 +3038,10 @@
         <v>16</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
@@ -3068,7 +3068,7 @@
         <v>62</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F13" s="22" t="s">
         <v>40</v>
@@ -3081,10 +3081,10 @@
         <v>16</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
@@ -3106,13 +3106,13 @@
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G14" s="22" t="str">
         <f t="shared" si="2"/>
@@ -3122,10 +3122,10 @@
         <v>16</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
@@ -3149,13 +3149,13 @@
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G15" s="22" t="str">
         <f t="shared" si="2"/>
@@ -3165,10 +3165,10 @@
         <v>16</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
@@ -3192,25 +3192,25 @@
       </c>
       <c r="C16" s="22"/>
       <c r="D16" s="22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E16" s="22"/>
       <c r="F16" s="22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G16" s="22" t="str">
         <f t="shared" si="2"/>
         <v>0000001001</v>
       </c>
       <c r="H16" s="22" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I16" s="22"/>
       <c r="J16" s="22" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K16" s="22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L16" s="22"/>
       <c r="M16" s="22"/>
@@ -3231,21 +3231,21 @@
       </c>
       <c r="C17" s="35"/>
       <c r="D17" s="35" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E17" s="35"/>
       <c r="F17" s="35" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G17" s="35" t="str">
         <f t="shared" si="2"/>
         <v>0000001010</v>
       </c>
       <c r="H17" s="35" t="s">
+        <v>398</v>
+      </c>
+      <c r="I17" s="35" t="s">
         <v>399</v>
-      </c>
-      <c r="I17" s="35" t="s">
-        <v>400</v>
       </c>
       <c r="J17" s="35"/>
       <c r="K17" s="35"/>
@@ -3268,21 +3268,21 @@
       </c>
       <c r="C18" s="35"/>
       <c r="D18" s="35" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E18" s="35"/>
       <c r="F18" s="35" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G18" s="35" t="str">
         <f t="shared" si="2"/>
         <v>0000001011</v>
       </c>
       <c r="H18" s="35" t="s">
+        <v>398</v>
+      </c>
+      <c r="I18" s="35" t="s">
         <v>399</v>
-      </c>
-      <c r="I18" s="35" t="s">
-        <v>400</v>
       </c>
       <c r="J18" s="35"/>
       <c r="K18" s="35"/>
@@ -3334,22 +3334,22 @@
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E20" s="22"/>
       <c r="F20" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G20" s="6" t="str">
         <f t="shared" si="2"/>
         <v>0000001101</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I20" s="6"/>
       <c r="J20" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
@@ -3369,26 +3369,26 @@
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>282</v>
+      </c>
+      <c r="F21" s="6" t="s">
         <v>177</v>
-      </c>
-      <c r="E21" s="22" t="s">
-        <v>283</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>178</v>
       </c>
       <c r="G21" s="6" t="str">
         <f t="shared" si="2"/>
         <v>0000001110</v>
       </c>
       <c r="H21" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="I21" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="J21" s="6" t="s">
         <v>180</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>181</v>
       </c>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
@@ -3435,22 +3435,22 @@
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E23" s="22"/>
       <c r="F23" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G23" s="6" t="str">
         <f t="shared" si="2"/>
         <v>0000010000</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I23" s="6"/>
       <c r="J23" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
@@ -3470,22 +3470,22 @@
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E24" s="22"/>
       <c r="F24" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G24" s="6" t="str">
         <f t="shared" si="2"/>
         <v>0000010001</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I24" s="6"/>
       <c r="J24" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
@@ -3532,27 +3532,27 @@
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G26" s="6" t="str">
         <f t="shared" si="2"/>
         <v>0000010011</v>
       </c>
       <c r="H26" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="I26" s="6" t="s">
         <v>347</v>
       </c>
-      <c r="I26" s="6" t="s">
+      <c r="J26" s="6" t="s">
         <v>348</v>
       </c>
-      <c r="J26" s="6" t="s">
-        <v>349</v>
-      </c>
       <c r="K26" s="6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
@@ -3571,27 +3571,27 @@
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G27" s="6" t="str">
         <f t="shared" si="2"/>
         <v>0000010100</v>
       </c>
       <c r="H27" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="I27" s="6" t="s">
         <v>347</v>
       </c>
-      <c r="I27" s="6" t="s">
-        <v>348</v>
-      </c>
       <c r="J27" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="K27" s="6" t="s">
         <v>350</v>
-      </c>
-      <c r="K27" s="6" t="s">
-        <v>351</v>
       </c>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
@@ -3610,27 +3610,27 @@
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G28" s="6" t="str">
         <f>DEC2BIN(B28, 10)</f>
         <v>0000010101</v>
       </c>
       <c r="H28" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="I28" s="6" t="s">
         <v>347</v>
       </c>
-      <c r="I28" s="6" t="s">
+      <c r="J28" s="6" t="s">
         <v>348</v>
       </c>
-      <c r="J28" s="6" t="s">
-        <v>349</v>
-      </c>
       <c r="K28" s="6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
@@ -3649,27 +3649,27 @@
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G29" s="6" t="str">
         <f t="shared" si="2"/>
         <v>0000010110</v>
       </c>
       <c r="H29" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="I29" s="6" t="s">
         <v>347</v>
       </c>
-      <c r="I29" s="6" t="s">
-        <v>348</v>
-      </c>
       <c r="J29" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="K29" s="6" t="s">
         <v>350</v>
-      </c>
-      <c r="K29" s="6" t="s">
-        <v>351</v>
       </c>
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
@@ -3823,25 +3823,25 @@
       </c>
       <c r="C35" s="6"/>
       <c r="D35" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G35" s="6" t="str">
         <f t="shared" si="2"/>
         <v>0000011100</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I35" s="6"/>
       <c r="J35" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K35" s="35" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L35" s="35"/>
       <c r="M35" s="6"/>
@@ -3860,25 +3860,25 @@
       </c>
       <c r="C36" s="6"/>
       <c r="D36" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E36" s="6"/>
       <c r="F36" s="22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G36" s="6" t="str">
         <f t="shared" si="2"/>
         <v>0000011101</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I36" s="6"/>
       <c r="J36" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K36" s="35" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L36" s="35"/>
       <c r="M36" s="6"/>
@@ -3950,7 +3950,7 @@
         <v>32</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
@@ -4840,16 +4840,16 @@
         <v>0001000000</v>
       </c>
       <c r="H71" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I71" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J71" s="6" t="s">
         <v>97</v>
       </c>
       <c r="K71" s="32" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L71" s="32"/>
       <c r="M71" s="6"/>
@@ -4883,16 +4883,16 @@
         <v>0001000001</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I72" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J72" s="6" t="s">
         <v>98</v>
       </c>
       <c r="K72" s="32" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L72" s="32"/>
       <c r="M72" s="6"/>
@@ -4996,7 +4996,7 @@
       </c>
       <c r="C76" s="22"/>
       <c r="D76" s="22" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E76" s="22"/>
       <c r="F76" s="22" t="s">
@@ -5007,16 +5007,16 @@
         <v>0001000101</v>
       </c>
       <c r="H76" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I76" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J76" s="6" t="s">
         <v>99</v>
       </c>
       <c r="K76" s="32" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L76" s="32"/>
       <c r="M76" s="6"/>
@@ -5104,16 +5104,16 @@
         <v>0001001000</v>
       </c>
       <c r="H79" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I79" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J79" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K79" s="32" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L79" s="32"/>
       <c r="M79" s="6"/>
@@ -5147,16 +5147,16 @@
         <v>0001001001</v>
       </c>
       <c r="H80" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I80" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J80" s="6" t="s">
         <v>100</v>
       </c>
       <c r="K80" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L80" s="32"/>
       <c r="M80" s="6"/>
@@ -5897,11 +5897,11 @@
         <v>0001100011</v>
       </c>
       <c r="H106" s="22" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I106" s="22"/>
       <c r="J106" s="22" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="K106" s="6"/>
       <c r="L106" s="6"/>
@@ -6043,7 +6043,7 @@
       </c>
       <c r="I110" s="6"/>
       <c r="J110" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K110" s="6"/>
       <c r="L110" s="6"/>
@@ -6121,7 +6121,7 @@
       </c>
       <c r="E113" s="6"/>
       <c r="F113" s="22" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G113" s="8" t="str">
         <f t="shared" si="6"/>
@@ -6135,7 +6135,7 @@
         <v>107</v>
       </c>
       <c r="K113" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L113" s="10"/>
       <c r="M113" s="6"/>
@@ -6158,7 +6158,7 @@
       </c>
       <c r="E114" s="6"/>
       <c r="F114" s="22" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G114" s="8" t="str">
         <f t="shared" si="6"/>
@@ -6172,7 +6172,7 @@
         <v>108</v>
       </c>
       <c r="K114" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L114" s="10"/>
       <c r="M114" s="6"/>
@@ -6191,11 +6191,11 @@
       </c>
       <c r="C115" s="6"/>
       <c r="D115" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E115" s="6"/>
       <c r="F115" s="22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G115" s="8" t="str">
         <f t="shared" si="6"/>
@@ -6206,10 +6206,10 @@
         <v>69</v>
       </c>
       <c r="J115" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K115" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L115" s="10"/>
       <c r="M115" s="6"/>
@@ -6232,7 +6232,7 @@
       </c>
       <c r="E116" s="6"/>
       <c r="F116" s="22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G116" s="6" t="str">
         <f t="shared" si="6"/>
@@ -6243,10 +6243,10 @@
         <v>69</v>
       </c>
       <c r="J116" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K116" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L116" s="10"/>
       <c r="M116" s="6"/>
@@ -6272,7 +6272,7 @@
       </c>
       <c r="E117" s="6"/>
       <c r="F117" s="22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G117" s="6" t="str">
         <f t="shared" si="6"/>
@@ -6286,7 +6286,7 @@
         <v>109</v>
       </c>
       <c r="K117" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L117" s="10"/>
       <c r="M117" s="6"/>
@@ -6309,7 +6309,7 @@
       </c>
       <c r="E118" s="6"/>
       <c r="F118" s="22" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G118" s="6" t="str">
         <f t="shared" si="6"/>
@@ -6323,7 +6323,7 @@
         <v>110</v>
       </c>
       <c r="K118" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L118" s="10"/>
       <c r="M118" s="6"/>
@@ -6346,21 +6346,21 @@
       </c>
       <c r="E119" s="22"/>
       <c r="F119" s="22" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G119" s="22" t="str">
         <f t="shared" si="6"/>
         <v>0001110000</v>
       </c>
       <c r="H119" s="22" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I119" s="22"/>
       <c r="J119" s="22" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K119" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L119" s="10"/>
       <c r="M119" s="6"/>
@@ -6383,21 +6383,21 @@
       </c>
       <c r="E120" s="22"/>
       <c r="F120" s="22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G120" s="22" t="str">
         <f t="shared" si="6"/>
         <v>0001110001</v>
       </c>
       <c r="H120" s="22" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I120" s="22"/>
       <c r="J120" s="22" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K120" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L120" s="10"/>
       <c r="M120" s="6"/>
@@ -6420,23 +6420,23 @@
       </c>
       <c r="E121" s="6"/>
       <c r="F121" s="22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G121" s="6" t="str">
         <f t="shared" si="6"/>
         <v>0001110010</v>
       </c>
       <c r="H121" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I121" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J121" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K121" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L121" s="10"/>
       <c r="M121" s="6"/>
@@ -6459,23 +6459,23 @@
       </c>
       <c r="E122" s="6"/>
       <c r="F122" s="22" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G122" s="6" t="str">
         <f t="shared" si="6"/>
         <v>0001110011</v>
       </c>
       <c r="H122" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I122" s="6" t="s">
         <v>69</v>
       </c>
       <c r="J122" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="K122" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L122" s="10"/>
       <c r="M122" s="6"/>
@@ -6551,11 +6551,11 @@
       </c>
       <c r="C125" s="6"/>
       <c r="D125" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E125" s="6"/>
       <c r="F125" s="22" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G125" s="6" t="str">
         <f t="shared" si="6"/>
@@ -6563,13 +6563,13 @@
       </c>
       <c r="H125" s="6"/>
       <c r="I125" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J125" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K125" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L125" s="10"/>
       <c r="M125" s="6"/>
@@ -6588,11 +6588,11 @@
       </c>
       <c r="C126" s="6"/>
       <c r="D126" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E126" s="6"/>
       <c r="F126" s="22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G126" s="6" t="str">
         <f t="shared" si="6"/>
@@ -6600,13 +6600,13 @@
       </c>
       <c r="H126" s="6"/>
       <c r="I126" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J126" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K126" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L126" s="10"/>
       <c r="M126" s="6"/>
@@ -6679,11 +6679,11 @@
       </c>
       <c r="C129" s="6"/>
       <c r="D129" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E129" s="6"/>
       <c r="F129" s="22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G129" s="6" t="str">
         <f t="shared" si="6"/>
@@ -6691,10 +6691,10 @@
       </c>
       <c r="H129" s="6"/>
       <c r="I129" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J129" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K129" s="10"/>
       <c r="L129" s="10"/>
@@ -6727,7 +6727,7 @@
       <c r="I130" s="6"/>
       <c r="J130" s="6"/>
       <c r="K130" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L130" s="10"/>
       <c r="M130" s="6"/>
@@ -6853,14 +6853,14 @@
         <v>128</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D135" s="6" t="s">
         <v>38</v>
       </c>
       <c r="E135" s="6"/>
       <c r="F135" s="22" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G135" s="6" t="str">
         <f t="shared" si="6"/>
@@ -6870,19 +6870,19 @@
         <v>16</v>
       </c>
       <c r="I135" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J135" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K135" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L135" s="35" t="s">
+        <v>380</v>
+      </c>
+      <c r="M135" s="35" t="s">
         <v>381</v>
-      </c>
-      <c r="M135" s="35" t="s">
-        <v>382</v>
       </c>
       <c r="N135" s="24"/>
       <c r="O135" s="24">
@@ -6904,10 +6904,10 @@
       <c r="C136" s="6"/>
       <c r="D136" s="6"/>
       <c r="E136" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F136" s="22" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G136" s="6" t="str">
         <f t="shared" ref="G136:G199" si="10">DEC2BIN(B136, 10)</f>
@@ -6917,19 +6917,19 @@
         <v>16</v>
       </c>
       <c r="I136" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J136" s="22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K136" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L136" s="35" t="s">
+        <v>380</v>
+      </c>
+      <c r="M136" s="35" t="s">
         <v>381</v>
-      </c>
-      <c r="M136" s="35" t="s">
-        <v>382</v>
       </c>
       <c r="N136" s="24"/>
       <c r="O136" s="24">
@@ -6951,10 +6951,10 @@
       <c r="C137" s="6"/>
       <c r="D137" s="6"/>
       <c r="E137" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F137" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G137" s="6" t="str">
         <f t="shared" si="10"/>
@@ -6964,19 +6964,19 @@
         <v>16</v>
       </c>
       <c r="I137" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J137" s="22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K137" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L137" s="35" t="s">
+        <v>380</v>
+      </c>
+      <c r="M137" s="35" t="s">
         <v>381</v>
-      </c>
-      <c r="M137" s="35" t="s">
-        <v>382</v>
       </c>
       <c r="N137" s="24"/>
       <c r="O137" s="24">
@@ -7001,7 +7001,7 @@
       </c>
       <c r="E138" s="6"/>
       <c r="F138" s="22" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G138" s="6" t="str">
         <f t="shared" si="10"/>
@@ -7011,13 +7011,13 @@
         <v>16</v>
       </c>
       <c r="I138" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J138" s="22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K138" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L138" s="6"/>
       <c r="M138" s="6"/>
@@ -7041,10 +7041,10 @@
       <c r="C139" s="6"/>
       <c r="D139" s="6"/>
       <c r="E139" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F139" s="22" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G139" s="6" t="str">
         <f t="shared" si="10"/>
@@ -7054,13 +7054,13 @@
         <v>16</v>
       </c>
       <c r="I139" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J139" s="22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K139" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L139" s="6"/>
       <c r="M139" s="6"/>
@@ -7084,10 +7084,10 @@
       <c r="C140" s="6"/>
       <c r="D140" s="6"/>
       <c r="E140" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F140" s="22" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G140" s="6" t="str">
         <f t="shared" si="10"/>
@@ -7097,13 +7097,13 @@
         <v>16</v>
       </c>
       <c r="I140" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J140" s="22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K140" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L140" s="6"/>
       <c r="M140" s="6"/>
@@ -7183,7 +7183,7 @@
         <v>36</v>
       </c>
       <c r="E143" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F143" s="22" t="s">
         <v>30</v>
@@ -7196,13 +7196,13 @@
         <v>22</v>
       </c>
       <c r="I143" s="35" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="J143" s="6" t="s">
         <v>111</v>
       </c>
       <c r="K143" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L143" s="6"/>
       <c r="M143" s="6"/>
@@ -7229,7 +7229,7 @@
       </c>
       <c r="E144" s="6"/>
       <c r="F144" s="22" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G144" s="6" t="str">
         <f t="shared" ref="G144" si="11">DEC2BIN(B144, 10)</f>
@@ -7240,10 +7240,10 @@
       </c>
       <c r="I144" s="6"/>
       <c r="J144" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K144" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L144" s="6"/>
       <c r="M144" s="6"/>
@@ -7446,11 +7446,11 @@
         <v>112</v>
       </c>
       <c r="K151" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L151" s="6"/>
       <c r="M151" s="35" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="N151" s="24"/>
       <c r="O151" s="24">
@@ -7714,28 +7714,28 @@
       </c>
       <c r="C161" s="27"/>
       <c r="D161" s="27" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E161" s="27"/>
       <c r="F161" s="28" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G161" s="27" t="str">
         <f t="shared" si="10"/>
         <v>0010011010</v>
       </c>
       <c r="H161" s="27" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I161" s="27"/>
       <c r="J161" s="22" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="K161" s="22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L161" s="22" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="M161" s="22"/>
       <c r="N161" s="30"/>
@@ -7757,30 +7757,30 @@
       </c>
       <c r="C162" s="27"/>
       <c r="D162" s="27" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E162" s="27" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F162" s="28" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G162" s="27" t="str">
         <f t="shared" si="10"/>
         <v>0010011011</v>
       </c>
       <c r="H162" s="27" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I162" s="27"/>
       <c r="J162" s="22" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="K162" s="22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L162" s="22" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="M162" s="22"/>
       <c r="N162" s="30"/>
@@ -7802,30 +7802,30 @@
       </c>
       <c r="C163" s="27"/>
       <c r="D163" s="27" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E163" s="27" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F163" s="28" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G163" s="27" t="str">
         <f t="shared" si="10"/>
         <v>0010011100</v>
       </c>
       <c r="H163" s="27" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I163" s="27"/>
       <c r="J163" s="22" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="K163" s="22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L163" s="22" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M163" s="22"/>
       <c r="N163" s="30"/>
@@ -7847,25 +7847,25 @@
       </c>
       <c r="C164" s="27"/>
       <c r="D164" s="27" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E164" s="27"/>
       <c r="F164" s="28" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G164" s="27" t="str">
         <f t="shared" si="10"/>
         <v>0010011101</v>
       </c>
       <c r="H164" s="27" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I164" s="27"/>
       <c r="J164" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K164" s="22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L164" s="22"/>
       <c r="M164" s="22"/>
@@ -7888,27 +7888,27 @@
       </c>
       <c r="C165" s="27"/>
       <c r="D165" s="27" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E165" s="27" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F165" s="28" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G165" s="27" t="str">
         <f t="shared" si="10"/>
         <v>0010011110</v>
       </c>
       <c r="H165" s="27" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I165" s="27"/>
       <c r="J165" s="22" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="K165" s="22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L165" s="22"/>
       <c r="M165" s="22"/>
@@ -7931,27 +7931,27 @@
       </c>
       <c r="C166" s="27"/>
       <c r="D166" s="27" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E166" s="27" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F166" s="28" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G166" s="27" t="str">
         <f t="shared" si="10"/>
         <v>0010011111</v>
       </c>
       <c r="H166" s="27" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I166" s="27"/>
       <c r="J166" s="22" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="K166" s="22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L166" s="22"/>
       <c r="M166" s="22"/>
@@ -7979,10 +7979,10 @@
         <v>73</v>
       </c>
       <c r="E167" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F167" s="28" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G167" s="6" t="str">
         <f t="shared" si="10"/>
@@ -7992,13 +7992,13 @@
         <v>120</v>
       </c>
       <c r="I167" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J167" s="6" t="s">
         <v>113</v>
       </c>
       <c r="K167" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L167" s="6"/>
       <c r="M167" s="6"/>
@@ -8010,7 +8010,7 @@
         <v>94</v>
       </c>
       <c r="Q167" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="168" spans="1:17" x14ac:dyDescent="0.15">
@@ -8026,10 +8026,10 @@
         <v>74</v>
       </c>
       <c r="E168" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F168" s="22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G168" s="6" t="str">
         <f t="shared" si="10"/>
@@ -8039,13 +8039,13 @@
         <v>120</v>
       </c>
       <c r="I168" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J168" s="6" t="s">
         <v>114</v>
       </c>
       <c r="K168" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L168" s="6"/>
       <c r="M168" s="6"/>
@@ -8057,7 +8057,7 @@
         <v>94</v>
       </c>
       <c r="Q168" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="169" spans="1:17" x14ac:dyDescent="0.15">
@@ -8073,10 +8073,10 @@
         <v>75</v>
       </c>
       <c r="E169" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F169" s="22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G169" s="6" t="str">
         <f t="shared" si="10"/>
@@ -8086,13 +8086,13 @@
         <v>120</v>
       </c>
       <c r="I169" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J169" s="6" t="s">
         <v>115</v>
       </c>
       <c r="K169" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L169" s="6"/>
       <c r="M169" s="6"/>
@@ -8104,7 +8104,7 @@
         <v>94</v>
       </c>
       <c r="Q169" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="170" spans="1:17" x14ac:dyDescent="0.15">
@@ -8117,27 +8117,27 @@
       </c>
       <c r="C170" s="6"/>
       <c r="D170" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E170" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F170" s="22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G170" s="6" t="str">
         <f t="shared" si="10"/>
         <v>0010100011</v>
       </c>
       <c r="H170" s="9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I170" s="9"/>
       <c r="J170" s="6" t="s">
         <v>115</v>
       </c>
       <c r="K170" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L170" s="6"/>
       <c r="M170" s="6"/>
@@ -8149,7 +8149,7 @@
         <v>94</v>
       </c>
       <c r="Q170" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="171" spans="1:17" x14ac:dyDescent="0.15">
@@ -8489,10 +8489,10 @@
         <v>73</v>
       </c>
       <c r="E183" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F183" s="28" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G183" s="6" t="str">
         <f t="shared" si="10"/>
@@ -8502,13 +8502,13 @@
         <v>120</v>
       </c>
       <c r="I183" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J183" s="6" t="s">
         <v>113</v>
       </c>
       <c r="K183" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L183" s="6"/>
       <c r="M183" s="6"/>
@@ -8520,7 +8520,7 @@
         <v>94</v>
       </c>
       <c r="Q183" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="184" spans="1:17" x14ac:dyDescent="0.15">
@@ -8536,10 +8536,10 @@
         <v>74</v>
       </c>
       <c r="E184" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F184" s="22" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G184" s="6" t="str">
         <f t="shared" si="10"/>
@@ -8549,13 +8549,13 @@
         <v>120</v>
       </c>
       <c r="I184" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J184" s="6" t="s">
         <v>114</v>
       </c>
       <c r="K184" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L184" s="6"/>
       <c r="M184" s="6"/>
@@ -8567,7 +8567,7 @@
         <v>94</v>
       </c>
       <c r="Q184" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="185" spans="1:17" x14ac:dyDescent="0.15">
@@ -8583,10 +8583,10 @@
         <v>75</v>
       </c>
       <c r="E185" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F185" s="22" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G185" s="6" t="str">
         <f t="shared" si="10"/>
@@ -8596,13 +8596,13 @@
         <v>120</v>
       </c>
       <c r="I185" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J185" s="6" t="s">
         <v>115</v>
       </c>
       <c r="K185" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L185" s="6"/>
       <c r="M185" s="6"/>
@@ -8614,7 +8614,7 @@
         <v>94</v>
       </c>
       <c r="Q185" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="186" spans="1:17" x14ac:dyDescent="0.15">
@@ -8984,7 +8984,7 @@
       </c>
       <c r="E199" s="6"/>
       <c r="F199" s="22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G199" s="6" t="str">
         <f t="shared" si="10"/>
@@ -8998,7 +8998,7 @@
         <v>116</v>
       </c>
       <c r="K199" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L199" s="6"/>
       <c r="M199" s="22"/>
@@ -9021,7 +9021,7 @@
       </c>
       <c r="E200" s="6"/>
       <c r="F200" s="22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G200" s="6" t="str">
         <f t="shared" ref="G200:G201" si="15">DEC2BIN(B200, 10)</f>
@@ -9035,7 +9035,7 @@
         <v>117</v>
       </c>
       <c r="K200" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L200" s="6"/>
       <c r="M200" s="10"/>
@@ -9058,7 +9058,7 @@
       </c>
       <c r="E201" s="6"/>
       <c r="F201" s="22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G201" s="6" t="str">
         <f t="shared" si="15"/>
@@ -9069,10 +9069,10 @@
       </c>
       <c r="I201" s="6"/>
       <c r="J201" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K201" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L201" s="6"/>
       <c r="M201" s="6"/>
@@ -9091,11 +9091,11 @@
       </c>
       <c r="C202" s="6"/>
       <c r="D202" s="22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E202" s="22"/>
       <c r="F202" s="22" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G202" s="6" t="str">
         <f t="shared" ref="G202:G208" si="16">DEC2BIN(B202, 10)</f>
@@ -9106,10 +9106,10 @@
       </c>
       <c r="I202" s="6"/>
       <c r="J202" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K202" s="35" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L202" s="35"/>
       <c r="M202" s="10"/>
@@ -9128,11 +9128,11 @@
       </c>
       <c r="C203" s="6"/>
       <c r="D203" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E203" s="6"/>
       <c r="F203" s="22" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G203" s="6" t="str">
         <f t="shared" si="16"/>
@@ -9143,10 +9143,10 @@
       </c>
       <c r="I203" s="6"/>
       <c r="J203" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K203" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L203" s="6"/>
       <c r="M203" s="6"/>
@@ -9169,7 +9169,7 @@
       </c>
       <c r="E204" s="22"/>
       <c r="F204" s="22" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G204" s="6" t="str">
         <f t="shared" si="16"/>
@@ -9180,10 +9180,10 @@
       </c>
       <c r="I204" s="6"/>
       <c r="J204" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="K204" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L204" s="6"/>
       <c r="M204" s="6"/>
@@ -9258,11 +9258,11 @@
       </c>
       <c r="C207" s="6"/>
       <c r="D207" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E207" s="6"/>
       <c r="F207" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G207" s="6" t="str">
         <f t="shared" si="16"/>
@@ -9273,15 +9273,15 @@
       </c>
       <c r="I207" s="6"/>
       <c r="J207" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K207" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L207" s="6"/>
       <c r="M207" s="10"/>
       <c r="N207" s="24" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O207" s="24">
         <v>3</v>
@@ -9305,7 +9305,7 @@
       </c>
       <c r="E208" s="6"/>
       <c r="F208" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G208" s="6" t="str">
         <f t="shared" si="16"/>
@@ -9319,12 +9319,12 @@
         <v>118</v>
       </c>
       <c r="K208" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L208" s="6"/>
       <c r="M208" s="6"/>
       <c r="N208" s="24" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O208" s="24">
         <v>3</v>
@@ -9344,25 +9344,25 @@
       </c>
       <c r="C209" s="6"/>
       <c r="D209" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E209" s="6"/>
       <c r="F209" s="22" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G209" s="6" t="str">
         <f t="shared" ref="G209:G262" si="17">DEC2BIN(B209, 10)</f>
         <v>0011001010</v>
       </c>
       <c r="H209" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I209" s="6"/>
       <c r="J209" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K209" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L209" s="6"/>
       <c r="M209" s="6"/>
@@ -9370,7 +9370,7 @@
       <c r="O209" s="24"/>
       <c r="P209" s="24"/>
       <c r="Q209" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="210" spans="1:17" x14ac:dyDescent="0.15">
@@ -9383,25 +9383,25 @@
       </c>
       <c r="C210" s="6"/>
       <c r="D210" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E210" s="6"/>
       <c r="F210" s="22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G210" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011001011</v>
       </c>
       <c r="H210" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I210" s="6"/>
       <c r="J210" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="K210" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L210" s="6"/>
       <c r="M210" s="6"/>
@@ -9420,25 +9420,25 @@
       </c>
       <c r="C211" s="6"/>
       <c r="D211" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E211" s="6"/>
       <c r="F211" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G211" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011001100</v>
       </c>
       <c r="H211" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I211" s="6"/>
       <c r="J211" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K211" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L211" s="6"/>
       <c r="M211" s="6"/>
@@ -9457,11 +9457,11 @@
       </c>
       <c r="C212" s="6"/>
       <c r="D212" s="34" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E212" s="34"/>
       <c r="F212" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G212" s="6" t="str">
         <f t="shared" si="17"/>
@@ -9473,7 +9473,7 @@
       <c r="I212" s="6"/>
       <c r="J212" s="6"/>
       <c r="K212" s="35" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L212" s="35"/>
       <c r="M212" s="6"/>
@@ -9492,11 +9492,11 @@
       </c>
       <c r="C213" s="6"/>
       <c r="D213" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E213" s="6"/>
       <c r="F213" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G213" s="6" t="str">
         <f t="shared" si="17"/>
@@ -9508,7 +9508,7 @@
       <c r="I213" s="6"/>
       <c r="J213" s="6"/>
       <c r="K213" s="35" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L213" s="35"/>
       <c r="M213" s="6"/>
@@ -9556,11 +9556,11 @@
       </c>
       <c r="C215" s="6"/>
       <c r="D215" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E215" s="6"/>
       <c r="F215" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G215" s="6" t="str">
         <f t="shared" si="17"/>
@@ -9572,7 +9572,7 @@
       <c r="I215" s="6"/>
       <c r="J215" s="6"/>
       <c r="K215" s="35" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L215" s="35"/>
       <c r="M215" s="6"/>
@@ -9591,11 +9591,11 @@
       </c>
       <c r="C216" s="6"/>
       <c r="D216" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E216" s="6"/>
       <c r="F216" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G216" s="6" t="str">
         <f t="shared" si="17"/>
@@ -9607,7 +9607,7 @@
       <c r="I216" s="6"/>
       <c r="J216" s="6"/>
       <c r="K216" s="35" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L216" s="35"/>
       <c r="M216" s="6"/>
@@ -9653,23 +9653,23 @@
       </c>
       <c r="C218" s="22"/>
       <c r="D218" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E218" s="22"/>
       <c r="F218" s="22" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G218" s="22" t="str">
         <f t="shared" si="17"/>
         <v>0011010011</v>
       </c>
       <c r="H218" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I218" s="22"/>
       <c r="J218" s="22"/>
       <c r="K218" s="22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L218" s="22"/>
       <c r="M218" s="6"/>
@@ -9688,23 +9688,23 @@
       </c>
       <c r="C219" s="22"/>
       <c r="D219" s="22" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E219" s="22"/>
       <c r="F219" s="22" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G219" s="22" t="str">
         <f t="shared" si="17"/>
         <v>0011010100</v>
       </c>
       <c r="H219" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I219" s="22"/>
       <c r="J219" s="22"/>
       <c r="K219" s="22" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="L219" s="22"/>
       <c r="M219" s="6"/>
@@ -9723,23 +9723,23 @@
       </c>
       <c r="C220" s="22"/>
       <c r="D220" s="22" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E220" s="22"/>
       <c r="F220" s="22" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G220" s="22" t="str">
         <f t="shared" si="17"/>
         <v>0011010101</v>
       </c>
       <c r="H220" s="22" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I220" s="22"/>
       <c r="J220" s="22"/>
       <c r="K220" s="22" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="L220" s="22"/>
       <c r="M220" s="6"/>
@@ -9758,23 +9758,23 @@
       </c>
       <c r="C221" s="22"/>
       <c r="D221" s="22" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E221" s="22"/>
       <c r="F221" s="22" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G221" s="22" t="str">
         <f t="shared" si="17"/>
         <v>0011010110</v>
       </c>
       <c r="H221" s="22" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I221" s="22"/>
       <c r="J221" s="22"/>
       <c r="K221" s="22" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="L221" s="22"/>
       <c r="M221" s="6"/>
@@ -9793,25 +9793,25 @@
       </c>
       <c r="C222" s="32"/>
       <c r="D222" s="32" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E222" s="32"/>
       <c r="F222" s="32" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G222" s="32" t="str">
         <f t="shared" si="17"/>
         <v>0011010111</v>
       </c>
       <c r="H222" s="32" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I222" s="32"/>
       <c r="J222" s="32" t="s">
+        <v>335</v>
+      </c>
+      <c r="K222" s="32" t="s">
         <v>336</v>
-      </c>
-      <c r="K222" s="32" t="s">
-        <v>337</v>
       </c>
       <c r="L222" s="32"/>
       <c r="M222" s="6"/>
@@ -10052,7 +10052,7 @@
       </c>
       <c r="E231" s="6"/>
       <c r="F231" s="22" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G231" s="6" t="str">
         <f t="shared" si="17"/>
@@ -10066,7 +10066,7 @@
         <v>119</v>
       </c>
       <c r="K231" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L231" s="6"/>
       <c r="M231" s="6"/>
@@ -10085,11 +10085,11 @@
       </c>
       <c r="C232" s="32"/>
       <c r="D232" s="32" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E232" s="32"/>
       <c r="F232" s="32" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G232" s="32" t="str">
         <f t="shared" si="17"/>
@@ -10101,12 +10101,12 @@
       <c r="I232" s="32"/>
       <c r="J232" s="32"/>
       <c r="K232" s="32" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L232" s="32"/>
       <c r="M232" s="6"/>
       <c r="N232" s="24" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="O232" s="24"/>
       <c r="P232" s="24" t="s">
@@ -10134,7 +10134,7 @@
       <c r="I233" s="6"/>
       <c r="J233" s="6"/>
       <c r="K233" s="22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L233" s="22"/>
       <c r="M233" s="6"/>
@@ -10211,23 +10211,23 @@
       </c>
       <c r="E236" s="22"/>
       <c r="F236" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G236" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011100101</v>
       </c>
       <c r="H236" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I236" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J236" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="K236" s="22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L236" s="22"/>
       <c r="M236" s="6"/>
@@ -10308,11 +10308,11 @@
       </c>
       <c r="C239" s="6"/>
       <c r="D239" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E239" s="6"/>
       <c r="F239" s="22" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G239" s="6" t="str">
         <f>DEC2BIN(B239, 10)</f>
@@ -10323,10 +10323,10 @@
       </c>
       <c r="I239" s="6"/>
       <c r="J239" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K239" s="22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L239" s="22"/>
       <c r="M239" s="6"/>
@@ -10355,7 +10355,7 @@
       </c>
       <c r="E240" s="6"/>
       <c r="F240" s="22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G240" s="6" t="str">
         <f t="shared" si="17"/>
@@ -10366,10 +10366,10 @@
       </c>
       <c r="I240" s="6"/>
       <c r="J240" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K240" s="22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L240" s="22"/>
       <c r="M240" s="6"/>
@@ -10394,27 +10394,27 @@
       </c>
       <c r="C241" s="6"/>
       <c r="D241" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E241" s="6"/>
       <c r="F241" s="22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G241" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011101010</v>
       </c>
       <c r="H241" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I241" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J241" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="K241" s="22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L241" s="22"/>
       <c r="M241" s="6"/>
@@ -10428,7 +10428,7 @@
         <v>95</v>
       </c>
       <c r="Q241" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="242" spans="1:17" x14ac:dyDescent="0.15">
@@ -10495,11 +10495,11 @@
       </c>
       <c r="C244" s="6"/>
       <c r="D244" s="34" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E244" s="34"/>
       <c r="F244" s="6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G244" s="6" t="str">
         <f t="shared" si="17"/>
@@ -10511,7 +10511,7 @@
       <c r="I244" s="6"/>
       <c r="J244" s="6"/>
       <c r="K244" s="22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L244" s="22"/>
       <c r="M244" s="6"/>
@@ -10530,11 +10530,11 @@
       </c>
       <c r="C245" s="6"/>
       <c r="D245" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E245" s="6"/>
       <c r="F245" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G245" s="6" t="str">
         <f t="shared" si="17"/>
@@ -10546,7 +10546,7 @@
       <c r="I245" s="6"/>
       <c r="J245" s="6"/>
       <c r="K245" s="22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L245" s="22"/>
       <c r="M245" s="6"/>
@@ -10594,11 +10594,11 @@
       </c>
       <c r="C247" s="22"/>
       <c r="D247" s="22" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E247" s="22"/>
       <c r="F247" s="22" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G247" s="6" t="str">
         <f t="shared" si="17"/>
@@ -10610,7 +10610,7 @@
       <c r="I247" s="6"/>
       <c r="J247" s="6"/>
       <c r="K247" s="22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L247" s="22"/>
       <c r="M247" s="6"/>
@@ -10629,11 +10629,11 @@
       </c>
       <c r="C248" s="22"/>
       <c r="D248" s="22" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E248" s="22"/>
       <c r="F248" s="22" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G248" s="6" t="str">
         <f t="shared" si="17"/>
@@ -10645,7 +10645,7 @@
       <c r="I248" s="6"/>
       <c r="J248" s="6"/>
       <c r="K248" s="22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L248" s="22"/>
       <c r="M248" s="6"/>
@@ -10664,23 +10664,23 @@
       </c>
       <c r="C249" s="22"/>
       <c r="D249" s="22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E249" s="22"/>
       <c r="F249" s="22" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G249" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011110010</v>
       </c>
       <c r="H249" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I249" s="6"/>
       <c r="J249" s="6"/>
       <c r="K249" s="22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L249" s="22"/>
       <c r="M249" s="6"/>
@@ -10699,23 +10699,23 @@
       </c>
       <c r="C250" s="22"/>
       <c r="D250" s="22" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E250" s="22"/>
       <c r="F250" s="22" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G250" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011110011</v>
       </c>
       <c r="H250" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I250" s="6"/>
       <c r="J250" s="6"/>
       <c r="K250" s="22" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="L250" s="22"/>
       <c r="M250" s="6"/>
@@ -10734,23 +10734,23 @@
       </c>
       <c r="C251" s="22"/>
       <c r="D251" s="22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E251" s="22"/>
       <c r="F251" s="22" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G251" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011110100</v>
       </c>
       <c r="H251" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I251" s="6"/>
       <c r="J251" s="6"/>
       <c r="K251" s="22" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="L251" s="22"/>
       <c r="M251" s="6"/>
@@ -10769,23 +10769,23 @@
       </c>
       <c r="C252" s="22"/>
       <c r="D252" s="22" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E252" s="22"/>
       <c r="F252" s="22" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G252" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011110101</v>
       </c>
       <c r="H252" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I252" s="6"/>
       <c r="J252" s="6"/>
       <c r="K252" s="22" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="L252" s="22"/>
       <c r="M252" s="6"/>
@@ -10804,23 +10804,23 @@
       </c>
       <c r="C253" s="22"/>
       <c r="D253" s="22" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E253" s="22"/>
       <c r="F253" s="22" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G253" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011110110</v>
       </c>
       <c r="H253" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I253" s="6"/>
       <c r="J253" s="6"/>
       <c r="K253" s="22" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="L253" s="22"/>
       <c r="M253" s="6"/>
@@ -11055,13 +11055,13 @@
       </c>
       <c r="C262" s="35"/>
       <c r="D262" s="35" t="s">
+        <v>393</v>
+      </c>
+      <c r="E262" s="35" t="s">
+        <v>283</v>
+      </c>
+      <c r="F262" s="35" t="s">
         <v>394</v>
-      </c>
-      <c r="E262" s="35" t="s">
-        <v>284</v>
-      </c>
-      <c r="F262" s="35" t="s">
-        <v>395</v>
       </c>
       <c r="G262" s="35" t="str">
         <f t="shared" si="17"/>
@@ -11069,13 +11069,13 @@
       </c>
       <c r="H262" s="35"/>
       <c r="I262" s="35" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="J262" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="K262" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L262" s="6"/>
       <c r="M262" s="6"/>
@@ -11111,10 +11111,10 @@
       </c>
       <c r="I263" s="6"/>
       <c r="J263" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K263" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L263" s="6"/>
       <c r="M263" s="6"/>
@@ -11148,15 +11148,15 @@
       </c>
       <c r="I264" s="6"/>
       <c r="J264" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K264" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L264" s="6"/>
       <c r="M264" s="6"/>
       <c r="N264" s="24" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="O264" s="24">
         <v>3</v>
@@ -11191,10 +11191,10 @@
       </c>
       <c r="I265" s="6"/>
       <c r="J265" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K265" s="35" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L265" s="35"/>
       <c r="M265" s="6"/>
@@ -11213,29 +11213,29 @@
       </c>
       <c r="C266" s="6"/>
       <c r="D266" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E266" s="22" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F266" s="22" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G266" s="6" t="str">
         <f t="shared" ref="G266:G327" si="20">DEC2BIN(B266, 10)</f>
         <v>0100000011</v>
       </c>
       <c r="H266" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I266" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J266" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K266" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L266" s="6"/>
       <c r="M266" s="6"/>
@@ -12009,14 +12009,14 @@
         <v>288</v>
       </c>
       <c r="C295" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D295" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E295" s="6"/>
       <c r="F295" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G295" s="6" t="str">
         <f t="shared" si="20"/>
@@ -12024,13 +12024,13 @@
       </c>
       <c r="H295" s="6"/>
       <c r="I295" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="J295" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="J295" s="6" t="s">
-        <v>224</v>
-      </c>
       <c r="K295" s="35" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L295" s="35"/>
       <c r="M295" s="6"/>
@@ -12049,27 +12049,27 @@
       </c>
       <c r="C296" s="6"/>
       <c r="D296" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E296" s="6"/>
       <c r="F296" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G296" s="6" t="str">
         <f t="shared" si="20"/>
         <v>0100100001</v>
       </c>
       <c r="H296" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="I296" s="6" t="s">
         <v>406</v>
       </c>
-      <c r="I296" s="6" t="s">
+      <c r="J296" s="6" t="s">
         <v>407</v>
       </c>
-      <c r="J296" s="6" t="s">
-        <v>408</v>
-      </c>
       <c r="K296" s="35" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L296" s="35"/>
       <c r="M296" s="6"/>
@@ -12088,37 +12088,37 @@
       </c>
       <c r="C297" s="6"/>
       <c r="D297" s="27" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E297" s="28"/>
       <c r="F297" s="28" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G297" s="28" t="str">
         <f t="shared" si="20"/>
         <v>0100100010</v>
       </c>
       <c r="H297" s="28" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I297" s="28"/>
       <c r="J297" s="28" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K297" s="28" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L297" s="28"/>
       <c r="M297" s="28"/>
       <c r="N297" s="39" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="O297" s="39"/>
       <c r="P297" s="39" t="s">
+        <v>293</v>
+      </c>
+      <c r="Q297" s="40" t="s">
         <v>294</v>
-      </c>
-      <c r="Q297" s="40" t="s">
-        <v>295</v>
       </c>
       <c r="R297" s="41"/>
     </row>
@@ -12132,11 +12132,11 @@
       </c>
       <c r="C298" s="6"/>
       <c r="D298" s="6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E298" s="6"/>
       <c r="F298" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G298" s="6" t="str">
         <f t="shared" si="20"/>
@@ -12163,11 +12163,11 @@
       </c>
       <c r="C299" s="6"/>
       <c r="D299" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E299" s="6"/>
       <c r="F299" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G299" s="6" t="str">
         <f t="shared" si="20"/>

</xml_diff>

<commit_message>
Add instrudtions : srif0r, srif1r
</commit_message>
<xml_diff>
--- a/instructions/mist32_isa.xlsx
+++ b/instructions/mist32_isa.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="418">
   <si>
     <t>ADD</t>
     <phoneticPr fontId="1"/>
@@ -1924,6 +1924,41 @@
   </si>
   <si>
     <t>Note</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SRFI0R</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SRFI1R</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>O1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Rd = FI0R</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Rd = FI1R</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>フラグを発生しない</t>
+    <rPh sb="4" eb="6">
+      <t>ハッセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FI1R Read</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FI0R Read</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2690,8 +2725,8 @@
   </sheetPr>
   <dimension ref="A2:AK1031"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I127" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I129" sqref="I129"/>
+    <sheetView tabSelected="1" topLeftCell="A190" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D215" sqref="D215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9808,17 +9843,27 @@
         <v>216</v>
       </c>
       <c r="C223" s="6"/>
-      <c r="D223" s="6"/>
+      <c r="D223" s="6" t="s">
+        <v>417</v>
+      </c>
       <c r="E223" s="6"/>
-      <c r="F223" s="6"/>
+      <c r="F223" s="6" t="s">
+        <v>410</v>
+      </c>
       <c r="G223" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011011000</v>
       </c>
-      <c r="H223" s="6"/>
+      <c r="H223" s="6" t="s">
+        <v>412</v>
+      </c>
       <c r="I223" s="6"/>
-      <c r="J223" s="6"/>
-      <c r="K223" s="6"/>
+      <c r="J223" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="K223" s="6" t="s">
+        <v>415</v>
+      </c>
       <c r="L223" s="6"/>
       <c r="M223" s="6"/>
       <c r="N223" s="24"/>
@@ -9835,17 +9880,27 @@
         <v>217</v>
       </c>
       <c r="C224" s="6"/>
-      <c r="D224" s="6"/>
+      <c r="D224" s="6" t="s">
+        <v>416</v>
+      </c>
       <c r="E224" s="6"/>
-      <c r="F224" s="6"/>
+      <c r="F224" s="6" t="s">
+        <v>411</v>
+      </c>
       <c r="G224" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011011001</v>
       </c>
-      <c r="H224" s="6"/>
+      <c r="H224" s="6" t="s">
+        <v>412</v>
+      </c>
       <c r="I224" s="6"/>
-      <c r="J224" s="6"/>
-      <c r="K224" s="6"/>
+      <c r="J224" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="K224" s="6" t="s">
+        <v>415</v>
+      </c>
       <c r="L224" s="6"/>
       <c r="M224" s="6"/>
       <c r="N224" s="24"/>

</xml_diff>

<commit_message>
Add description : Load/Store with displacement(LDD8, LDD16, LDD32, STD8, STD16, STD32)
</commit_message>
<xml_diff>
--- a/instructions/mist32_isa.xlsx
+++ b/instructions/mist32_isa.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="422">
   <si>
     <t>ADD</t>
     <phoneticPr fontId="1"/>
@@ -1727,10 +1727,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Rd = mask(MEMORY[Rs+displacement], 8)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Rd = mask(MEMORY[Rs+displacement], 16)</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1748,10 +1744,6 @@
   </si>
   <si>
     <t>Instruction</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Immediate</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1959,6 +1951,38 @@
   </si>
   <si>
     <t>FI0R Read</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Rd = mask(MEMORY[Rs+displacement], 8)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Immediate(Displacement)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>(符号拡張)</t>
+  </si>
+  <si>
+    <t>(符号拡張)</t>
+    <rPh sb="1" eb="5">
+      <t>フゴウカクチョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1bit左シフト(符号拡張・1bit左シフト)</t>
+    <rPh sb="4" eb="5">
+      <t>ヒダリ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2bit左シフト(符号拡張・2bit左シフト)</t>
+    <rPh sb="4" eb="5">
+      <t>ヒダリ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2725,8 +2749,8 @@
   </sheetPr>
   <dimension ref="A2:AK1031"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D215" sqref="D215"/>
+    <sheetView tabSelected="1" topLeftCell="B136" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D165" sqref="D165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2735,7 +2759,7 @@
     <col min="2" max="2" width="6.125" customWidth="1"/>
     <col min="3" max="3" width="19.25" customWidth="1"/>
     <col min="4" max="4" width="55.375" customWidth="1"/>
-    <col min="5" max="5" width="28" customWidth="1"/>
+    <col min="5" max="5" width="34.625" customWidth="1"/>
     <col min="6" max="6" width="40.875" customWidth="1"/>
     <col min="7" max="7" width="11.25" customWidth="1"/>
     <col min="8" max="8" width="20.125" customWidth="1"/>
@@ -2778,55 +2802,55 @@
     </row>
     <row r="6" spans="1:19" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B6" s="18" t="s">
+        <v>391</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>365</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>417</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>367</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>368</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>400</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>401</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>369</v>
+      </c>
+      <c r="K6" s="18" t="s">
         <v>393</v>
       </c>
-      <c r="C6" s="18" t="s">
-        <v>366</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>367</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>368</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>369</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>370</v>
-      </c>
-      <c r="H6" s="18" t="s">
+      <c r="L6" s="29" t="s">
         <v>402</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="M6" s="43" t="s">
         <v>403</v>
       </c>
-      <c r="J6" s="18" t="s">
-        <v>371</v>
-      </c>
-      <c r="K6" s="18" t="s">
-        <v>395</v>
-      </c>
-      <c r="L6" s="29" t="s">
+      <c r="N6" s="26" t="s">
         <v>404</v>
       </c>
-      <c r="M6" s="43" t="s">
+      <c r="O6" s="33" t="s">
         <v>405</v>
       </c>
-      <c r="N6" s="26" t="s">
+      <c r="P6" s="33" t="s">
         <v>406</v>
       </c>
-      <c r="O6" s="33" t="s">
+      <c r="Q6" s="19" t="s">
         <v>407</v>
-      </c>
-      <c r="P6" s="33" t="s">
-        <v>408</v>
-      </c>
-      <c r="Q6" s="19" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
@@ -2938,7 +2962,7 @@
         <v>144</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
@@ -2977,7 +3001,7 @@
         <v>144</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
@@ -3245,21 +3269,21 @@
       </c>
       <c r="C17" s="35"/>
       <c r="D17" s="35" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E17" s="35"/>
       <c r="F17" s="35" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="G17" s="35" t="str">
         <f t="shared" si="2"/>
         <v>0000001010</v>
       </c>
       <c r="H17" s="35" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="I17" s="35" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="J17" s="35"/>
       <c r="K17" s="35"/>
@@ -3282,21 +3306,21 @@
       </c>
       <c r="C18" s="35"/>
       <c r="D18" s="35" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E18" s="35"/>
       <c r="F18" s="35" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="G18" s="35" t="str">
         <f t="shared" si="2"/>
         <v>0000001011</v>
       </c>
       <c r="H18" s="35" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="I18" s="35" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="J18" s="35"/>
       <c r="K18" s="35"/>
@@ -3352,7 +3376,7 @@
       </c>
       <c r="E20" s="22"/>
       <c r="F20" s="6" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="G20" s="6" t="str">
         <f t="shared" si="2"/>
@@ -3964,7 +3988,7 @@
         <v>32</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
@@ -6867,7 +6891,7 @@
         <v>128</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D135" s="6" t="s">
         <v>38</v>
@@ -6893,10 +6917,10 @@
         <v>276</v>
       </c>
       <c r="L135" s="35" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="M135" s="35" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="N135" s="24"/>
       <c r="O135" s="24">
@@ -6940,10 +6964,10 @@
         <v>276</v>
       </c>
       <c r="L136" s="35" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="M136" s="35" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="N136" s="24"/>
       <c r="O136" s="24">
@@ -6987,10 +7011,10 @@
         <v>276</v>
       </c>
       <c r="L137" s="35" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="M137" s="35" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="N137" s="24"/>
       <c r="O137" s="24">
@@ -7197,7 +7221,7 @@
         <v>36</v>
       </c>
       <c r="E143" s="6" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F143" s="22" t="s">
         <v>30</v>
@@ -7210,7 +7234,7 @@
         <v>22</v>
       </c>
       <c r="I143" s="35" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="J143" s="6" t="s">
         <v>109</v>
@@ -7464,7 +7488,7 @@
       </c>
       <c r="L151" s="6"/>
       <c r="M151" s="35" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="N151" s="24"/>
       <c r="O151" s="24">
@@ -7728,9 +7752,11 @@
       </c>
       <c r="C161" s="27"/>
       <c r="D161" s="27" t="s">
-        <v>365</v>
-      </c>
-      <c r="E161" s="27"/>
+        <v>364</v>
+      </c>
+      <c r="E161" s="27" t="s">
+        <v>419</v>
+      </c>
       <c r="F161" s="28" t="s">
         <v>355</v>
       </c>
@@ -7743,13 +7769,13 @@
       </c>
       <c r="I161" s="27"/>
       <c r="J161" s="22" t="s">
-        <v>362</v>
+        <v>416</v>
       </c>
       <c r="K161" s="22" t="s">
         <v>276</v>
       </c>
       <c r="L161" s="22" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="M161" s="22"/>
       <c r="N161" s="30"/>
@@ -7771,10 +7797,10 @@
       </c>
       <c r="C162" s="27"/>
       <c r="D162" s="27" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E162" s="27" t="s">
-        <v>274</v>
+        <v>420</v>
       </c>
       <c r="F162" s="28" t="s">
         <v>356</v>
@@ -7788,13 +7814,13 @@
       </c>
       <c r="I162" s="27"/>
       <c r="J162" s="22" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K162" s="22" t="s">
         <v>276</v>
       </c>
       <c r="L162" s="22" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="M162" s="22"/>
       <c r="N162" s="30"/>
@@ -7816,10 +7842,10 @@
       </c>
       <c r="C163" s="27"/>
       <c r="D163" s="27" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E163" s="27" t="s">
-        <v>275</v>
+        <v>421</v>
       </c>
       <c r="F163" s="28" t="s">
         <v>357</v>
@@ -7833,13 +7859,13 @@
       </c>
       <c r="I163" s="27"/>
       <c r="J163" s="22" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K163" s="22" t="s">
         <v>276</v>
       </c>
       <c r="L163" s="22" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="M163" s="22"/>
       <c r="N163" s="30"/>
@@ -7861,9 +7887,11 @@
       </c>
       <c r="C164" s="27"/>
       <c r="D164" s="27" t="s">
-        <v>365</v>
-      </c>
-      <c r="E164" s="27"/>
+        <v>364</v>
+      </c>
+      <c r="E164" s="27" t="s">
+        <v>418</v>
+      </c>
       <c r="F164" s="28" t="s">
         <v>358</v>
       </c>
@@ -7902,10 +7930,10 @@
       </c>
       <c r="C165" s="27"/>
       <c r="D165" s="27" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E165" s="27" t="s">
-        <v>274</v>
+        <v>420</v>
       </c>
       <c r="F165" s="28" t="s">
         <v>359</v>
@@ -7919,7 +7947,7 @@
       </c>
       <c r="I165" s="27"/>
       <c r="J165" s="22" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="K165" s="22" t="s">
         <v>276</v>
@@ -7945,10 +7973,10 @@
       </c>
       <c r="C166" s="27"/>
       <c r="D166" s="27" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E166" s="27" t="s">
-        <v>275</v>
+        <v>421</v>
       </c>
       <c r="F166" s="28" t="s">
         <v>360</v>
@@ -7962,7 +7990,7 @@
       </c>
       <c r="I166" s="27"/>
       <c r="J166" s="22" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="K166" s="22" t="s">
         <v>276</v>
@@ -9844,25 +9872,25 @@
       </c>
       <c r="C223" s="6"/>
       <c r="D223" s="6" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E223" s="6"/>
       <c r="F223" s="6" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="G223" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011011000</v>
       </c>
       <c r="H223" s="6" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="I223" s="6"/>
       <c r="J223" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="K223" s="6" t="s">
         <v>413</v>
-      </c>
-      <c r="K223" s="6" t="s">
-        <v>415</v>
       </c>
       <c r="L223" s="6"/>
       <c r="M223" s="6"/>
@@ -9881,25 +9909,25 @@
       </c>
       <c r="C224" s="6"/>
       <c r="D224" s="6" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E224" s="6"/>
       <c r="F224" s="6" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="G224" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011011001</v>
       </c>
       <c r="H224" s="6" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="I224" s="6"/>
       <c r="J224" s="6" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="K224" s="6" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="L224" s="6"/>
       <c r="M224" s="6"/>
@@ -10803,7 +10831,7 @@
       </c>
       <c r="C252" s="22"/>
       <c r="D252" s="22" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E252" s="22"/>
       <c r="F252" s="22" t="s">
@@ -10838,7 +10866,7 @@
       </c>
       <c r="C253" s="22"/>
       <c r="D253" s="22" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E253" s="22"/>
       <c r="F253" s="22" t="s">
@@ -11089,13 +11117,13 @@
       </c>
       <c r="C262" s="35"/>
       <c r="D262" s="35" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E262" s="35" t="s">
         <v>278</v>
       </c>
       <c r="F262" s="35" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="G262" s="35" t="str">
         <f t="shared" si="17"/>
@@ -11103,10 +11131,10 @@
       </c>
       <c r="H262" s="35"/>
       <c r="I262" s="35" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="J262" s="6" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="K262" s="6" t="s">
         <v>276</v>
@@ -11190,7 +11218,7 @@
       <c r="L264" s="6"/>
       <c r="M264" s="6"/>
       <c r="N264" s="24" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="O264" s="24">
         <v>3</v>
@@ -12094,13 +12122,13 @@
         <v>0100100001</v>
       </c>
       <c r="H296" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="I296" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="J296" s="6" t="s">
         <v>396</v>
-      </c>
-      <c r="I296" s="6" t="s">
-        <v>397</v>
-      </c>
-      <c r="J296" s="6" t="s">
-        <v>398</v>
       </c>
       <c r="K296" s="35" t="s">
         <v>276</v>

</xml_diff>

<commit_message>
added : ld8u, ;ld16u, ld32u, st8u, ;st16u, st32u
</commit_message>
<xml_diff>
--- a/instructions/mist32_isa.xlsx
+++ b/instructions/mist32_isa.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="435">
   <si>
     <t>ADD</t>
     <phoneticPr fontId="1"/>
@@ -165,10 +165,6 @@
   </si>
   <si>
     <t>set word</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>push</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1982,6 +1978,73 @@
     <t>2bit左シフト(符号拡張・2bit左シフト)</t>
     <rPh sb="4" eb="5">
       <t>ヒダリ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>push</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Load(always use PDTR)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Store(always use PDTR)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LD8U</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LD16U</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LD32U</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ST8U</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ST16U</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ST32U</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>O2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>I11</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2,3</t>
+  </si>
+  <si>
+    <t>2,3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メモリ保護違反、特権違反</t>
+    <rPh sb="3" eb="5">
+      <t>ホゴ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>イハン</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>トッケン</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>イハン</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -2749,8 +2812,8 @@
   </sheetPr>
   <dimension ref="A2:AK1031"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B136" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D165" sqref="D165"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J155" sqref="J155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2789,68 +2852,68 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.15">
       <c r="C3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="M5" s="44"/>
       <c r="N5" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O5" s="21"/>
       <c r="P5" s="21"/>
     </row>
     <row r="6" spans="1:19" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
+        <v>389</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>390</v>
       </c>
-      <c r="B6" s="18" t="s">
-        <v>391</v>
-      </c>
       <c r="C6" s="18" t="s">
+        <v>364</v>
+      </c>
+      <c r="D6" s="18" t="s">
         <v>365</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="E6" s="18" t="s">
+        <v>416</v>
+      </c>
+      <c r="F6" s="18" t="s">
         <v>366</v>
       </c>
-      <c r="E6" s="18" t="s">
-        <v>417</v>
-      </c>
-      <c r="F6" s="18" t="s">
+      <c r="G6" s="18" t="s">
         <v>367</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="H6" s="18" t="s">
+        <v>399</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>400</v>
+      </c>
+      <c r="J6" s="18" t="s">
         <v>368</v>
       </c>
-      <c r="H6" s="18" t="s">
-        <v>400</v>
-      </c>
-      <c r="I6" s="18" t="s">
+      <c r="K6" s="18" t="s">
+        <v>392</v>
+      </c>
+      <c r="L6" s="29" t="s">
         <v>401</v>
       </c>
-      <c r="J6" s="18" t="s">
-        <v>369</v>
-      </c>
-      <c r="K6" s="18" t="s">
-        <v>393</v>
-      </c>
-      <c r="L6" s="29" t="s">
+      <c r="M6" s="43" t="s">
         <v>402</v>
       </c>
-      <c r="M6" s="43" t="s">
+      <c r="N6" s="26" t="s">
         <v>403</v>
       </c>
-      <c r="N6" s="26" t="s">
+      <c r="O6" s="33" t="s">
         <v>404</v>
       </c>
-      <c r="O6" s="33" t="s">
+      <c r="P6" s="33" t="s">
         <v>405</v>
       </c>
-      <c r="P6" s="33" t="s">
+      <c r="Q6" s="19" t="s">
         <v>406</v>
-      </c>
-      <c r="Q6" s="19" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
@@ -2862,13 +2925,13 @@
         <v>0</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="38" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F7" s="15" t="s">
         <v>0</v>
@@ -2881,10 +2944,10 @@
         <v>16</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K7" s="15"/>
       <c r="L7" s="15"/>
@@ -2907,7 +2970,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>3</v>
@@ -2920,10 +2983,10 @@
         <v>16</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
@@ -2943,13 +3006,13 @@
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G9" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2959,10 +3022,10 @@
         <v>16</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
@@ -2982,13 +3045,13 @@
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G10" s="6" t="str">
         <f t="shared" ref="G10:G70" si="2">DEC2BIN(B10, 10)</f>
@@ -2998,10 +3061,10 @@
         <v>16</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
@@ -3021,11 +3084,11 @@
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E11" s="22"/>
       <c r="F11" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G11" s="6" t="str">
         <f t="shared" si="2"/>
@@ -3035,10 +3098,10 @@
         <v>16</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
@@ -3048,7 +3111,7 @@
         <v>4</v>
       </c>
       <c r="P11" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q11" s="7"/>
     </row>
@@ -3062,11 +3125,11 @@
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E12" s="22"/>
       <c r="F12" s="22" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G12" s="22" t="str">
         <f t="shared" si="2"/>
@@ -3076,10 +3139,10 @@
         <v>16</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
@@ -3089,7 +3152,7 @@
         <v>4</v>
       </c>
       <c r="P12" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q12" s="7"/>
     </row>
@@ -3103,13 +3166,13 @@
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G13" s="22" t="str">
         <f t="shared" si="2"/>
@@ -3119,10 +3182,10 @@
         <v>16</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
@@ -3131,7 +3194,7 @@
       <c r="O13" s="24"/>
       <c r="P13" s="24"/>
       <c r="Q13" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.15">
@@ -3144,13 +3207,13 @@
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G14" s="22" t="str">
         <f t="shared" si="2"/>
@@ -3160,10 +3223,10 @@
         <v>16</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
@@ -3173,7 +3236,7 @@
         <v>4</v>
       </c>
       <c r="P14" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q14" s="7"/>
     </row>
@@ -3187,13 +3250,13 @@
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G15" s="22" t="str">
         <f t="shared" si="2"/>
@@ -3203,10 +3266,10 @@
         <v>16</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
@@ -3216,7 +3279,7 @@
         <v>4</v>
       </c>
       <c r="P15" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q15" s="7"/>
     </row>
@@ -3230,25 +3293,25 @@
       </c>
       <c r="C16" s="22"/>
       <c r="D16" s="22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E16" s="22"/>
       <c r="F16" s="22" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G16" s="22" t="str">
         <f t="shared" si="2"/>
         <v>0000001001</v>
       </c>
       <c r="H16" s="22" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="I16" s="22"/>
       <c r="J16" s="22" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="K16" s="22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L16" s="22"/>
       <c r="M16" s="22"/>
@@ -3269,21 +3332,21 @@
       </c>
       <c r="C17" s="35"/>
       <c r="D17" s="35" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E17" s="35"/>
       <c r="F17" s="35" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G17" s="35" t="str">
         <f t="shared" si="2"/>
         <v>0000001010</v>
       </c>
       <c r="H17" s="35" t="s">
+        <v>386</v>
+      </c>
+      <c r="I17" s="35" t="s">
         <v>387</v>
-      </c>
-      <c r="I17" s="35" t="s">
-        <v>388</v>
       </c>
       <c r="J17" s="35"/>
       <c r="K17" s="35"/>
@@ -3306,21 +3369,21 @@
       </c>
       <c r="C18" s="35"/>
       <c r="D18" s="35" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E18" s="35"/>
       <c r="F18" s="35" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G18" s="35" t="str">
         <f t="shared" si="2"/>
         <v>0000001011</v>
       </c>
       <c r="H18" s="35" t="s">
+        <v>386</v>
+      </c>
+      <c r="I18" s="35" t="s">
         <v>387</v>
-      </c>
-      <c r="I18" s="35" t="s">
-        <v>388</v>
       </c>
       <c r="J18" s="35"/>
       <c r="K18" s="35"/>
@@ -3372,22 +3435,22 @@
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E20" s="22"/>
       <c r="F20" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G20" s="6" t="str">
         <f t="shared" si="2"/>
         <v>0000001101</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I20" s="6"/>
       <c r="J20" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
@@ -3407,26 +3470,26 @@
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>276</v>
+      </c>
+      <c r="F21" s="6" t="s">
         <v>172</v>
-      </c>
-      <c r="E21" s="22" t="s">
-        <v>277</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>173</v>
       </c>
       <c r="G21" s="6" t="str">
         <f t="shared" si="2"/>
         <v>0000001110</v>
       </c>
       <c r="H21" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="I21" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="J21" s="6" t="s">
         <v>175</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>176</v>
       </c>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
@@ -3473,22 +3536,22 @@
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E23" s="22"/>
       <c r="F23" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G23" s="6" t="str">
         <f t="shared" si="2"/>
         <v>0000010000</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I23" s="6"/>
       <c r="J23" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
@@ -3508,22 +3571,22 @@
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E24" s="22"/>
       <c r="F24" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G24" s="6" t="str">
         <f t="shared" si="2"/>
         <v>0000010001</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I24" s="6"/>
       <c r="J24" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
@@ -3570,27 +3633,27 @@
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G26" s="6" t="str">
         <f t="shared" si="2"/>
         <v>0000010011</v>
       </c>
       <c r="H26" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="I26" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="I26" s="6" t="s">
+      <c r="J26" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="J26" s="6" t="s">
-        <v>343</v>
-      </c>
       <c r="K26" s="6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
@@ -3609,27 +3672,27 @@
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G27" s="6" t="str">
         <f t="shared" si="2"/>
         <v>0000010100</v>
       </c>
       <c r="H27" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="I27" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="I27" s="6" t="s">
-        <v>342</v>
-      </c>
       <c r="J27" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="K27" s="6" t="s">
         <v>344</v>
-      </c>
-      <c r="K27" s="6" t="s">
-        <v>345</v>
       </c>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
@@ -3648,27 +3711,27 @@
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G28" s="6" t="str">
         <f>DEC2BIN(B28, 10)</f>
         <v>0000010101</v>
       </c>
       <c r="H28" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="I28" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="I28" s="6" t="s">
+      <c r="J28" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="J28" s="6" t="s">
-        <v>343</v>
-      </c>
       <c r="K28" s="6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
@@ -3687,27 +3750,27 @@
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G29" s="6" t="str">
         <f t="shared" si="2"/>
         <v>0000010110</v>
       </c>
       <c r="H29" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="I29" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="I29" s="6" t="s">
-        <v>342</v>
-      </c>
       <c r="J29" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="K29" s="6" t="s">
         <v>344</v>
-      </c>
-      <c r="K29" s="6" t="s">
-        <v>345</v>
       </c>
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
@@ -3861,25 +3924,25 @@
       </c>
       <c r="C35" s="6"/>
       <c r="D35" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G35" s="6" t="str">
         <f t="shared" si="2"/>
         <v>0000011100</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I35" s="6"/>
       <c r="J35" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K35" s="35" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L35" s="35"/>
       <c r="M35" s="6"/>
@@ -3898,25 +3961,25 @@
       </c>
       <c r="C36" s="6"/>
       <c r="D36" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E36" s="6"/>
       <c r="F36" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G36" s="6" t="str">
         <f t="shared" si="2"/>
         <v>0000011101</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I36" s="6"/>
       <c r="J36" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K36" s="35" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L36" s="35"/>
       <c r="M36" s="6"/>
@@ -3988,7 +4051,7 @@
         <v>32</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
@@ -4871,23 +4934,23 @@
       </c>
       <c r="E71" s="6"/>
       <c r="F71" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G71" s="6" t="str">
         <f t="shared" ref="G71:G82" si="3">DEC2BIN(B71, 10)</f>
         <v>0001000000</v>
       </c>
       <c r="H71" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I71" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J71" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K71" s="32" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L71" s="32"/>
       <c r="M71" s="6"/>
@@ -4896,7 +4959,7 @@
         <v>1</v>
       </c>
       <c r="P71" s="24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q71" s="7"/>
     </row>
@@ -4914,23 +4977,23 @@
       </c>
       <c r="E72" s="6"/>
       <c r="F72" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G72" s="6" t="str">
         <f t="shared" si="3"/>
         <v>0001000001</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I72" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J72" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K72" s="32" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L72" s="32"/>
       <c r="M72" s="6"/>
@@ -4939,7 +5002,7 @@
         <v>1</v>
       </c>
       <c r="P72" s="24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q72" s="7"/>
     </row>
@@ -5034,27 +5097,27 @@
       </c>
       <c r="C76" s="22"/>
       <c r="D76" s="22" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E76" s="22"/>
       <c r="F76" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G76" s="22" t="str">
         <f t="shared" si="3"/>
         <v>0001000101</v>
       </c>
       <c r="H76" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I76" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J76" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K76" s="32" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L76" s="32"/>
       <c r="M76" s="6"/>
@@ -5063,7 +5126,7 @@
         <v>1</v>
       </c>
       <c r="P76" s="24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q76" s="7"/>
     </row>
@@ -5135,23 +5198,23 @@
       </c>
       <c r="E79" s="22"/>
       <c r="F79" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G79" s="22" t="str">
         <f t="shared" si="3"/>
         <v>0001001000</v>
       </c>
       <c r="H79" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I79" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J79" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K79" s="32" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L79" s="32"/>
       <c r="M79" s="6"/>
@@ -5160,7 +5223,7 @@
         <v>1</v>
       </c>
       <c r="P79" s="24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q79" s="7"/>
     </row>
@@ -5178,23 +5241,23 @@
       </c>
       <c r="E80" s="22"/>
       <c r="F80" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G80" s="22" t="str">
         <f t="shared" si="3"/>
         <v>0001001001</v>
       </c>
       <c r="H80" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I80" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J80" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K80" s="32" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L80" s="32"/>
       <c r="M80" s="6"/>
@@ -5203,7 +5266,7 @@
         <v>1</v>
       </c>
       <c r="P80" s="24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q80" s="7"/>
     </row>
@@ -5831,7 +5894,7 @@
       </c>
       <c r="I103" s="6"/>
       <c r="J103" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K103" s="6"/>
       <c r="L103" s="6"/>
@@ -5866,7 +5929,7 @@
       </c>
       <c r="I104" s="22"/>
       <c r="J104" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K104" s="6"/>
       <c r="L104" s="6"/>
@@ -5889,22 +5952,22 @@
       </c>
       <c r="C105" s="6"/>
       <c r="D105" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E105" s="6"/>
       <c r="F105" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G105" s="6" t="str">
         <f t="shared" si="6"/>
         <v>0001100010</v>
       </c>
       <c r="H105" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I105" s="22"/>
       <c r="J105" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K105" s="6"/>
       <c r="L105" s="6"/>
@@ -5935,11 +5998,11 @@
         <v>0001100011</v>
       </c>
       <c r="H106" s="22" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="I106" s="22"/>
       <c r="J106" s="22" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K106" s="6"/>
       <c r="L106" s="6"/>
@@ -5974,7 +6037,7 @@
       </c>
       <c r="I107" s="6"/>
       <c r="J107" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K107" s="6"/>
       <c r="L107" s="6"/>
@@ -5995,11 +6058,11 @@
       </c>
       <c r="C108" s="6"/>
       <c r="D108" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E108" s="6"/>
       <c r="F108" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G108" s="6" t="str">
         <f t="shared" si="8"/>
@@ -6010,7 +6073,7 @@
       </c>
       <c r="I108" s="6"/>
       <c r="J108" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K108" s="6"/>
       <c r="L108" s="6"/>
@@ -6031,11 +6094,11 @@
       </c>
       <c r="C109" s="6"/>
       <c r="D109" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E109" s="6"/>
       <c r="F109" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G109" s="6" t="str">
         <f t="shared" si="8"/>
@@ -6046,7 +6109,7 @@
       </c>
       <c r="I109" s="6"/>
       <c r="J109" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K109" s="6"/>
       <c r="L109" s="6"/>
@@ -6066,22 +6129,22 @@
       </c>
       <c r="C110" s="6"/>
       <c r="D110" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E110" s="6"/>
       <c r="F110" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G110" s="6" t="str">
         <f t="shared" si="6"/>
         <v>0001100111</v>
       </c>
       <c r="H110" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I110" s="6"/>
       <c r="J110" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K110" s="6"/>
       <c r="L110" s="6"/>
@@ -6155,11 +6218,11 @@
       </c>
       <c r="C113" s="6"/>
       <c r="D113" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E113" s="6"/>
       <c r="F113" s="22" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G113" s="8" t="str">
         <f t="shared" si="6"/>
@@ -6170,10 +6233,10 @@
       </c>
       <c r="I113" s="6"/>
       <c r="J113" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K113" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L113" s="10"/>
       <c r="M113" s="6"/>
@@ -6192,11 +6255,11 @@
       </c>
       <c r="C114" s="6"/>
       <c r="D114" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E114" s="6"/>
       <c r="F114" s="22" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G114" s="8" t="str">
         <f t="shared" si="6"/>
@@ -6207,10 +6270,10 @@
       </c>
       <c r="I114" s="6"/>
       <c r="J114" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K114" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L114" s="10"/>
       <c r="M114" s="6"/>
@@ -6229,11 +6292,11 @@
       </c>
       <c r="C115" s="6"/>
       <c r="D115" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E115" s="6"/>
       <c r="F115" s="22" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G115" s="8" t="str">
         <f t="shared" si="6"/>
@@ -6241,13 +6304,13 @@
       </c>
       <c r="H115" s="6"/>
       <c r="I115" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J115" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K115" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L115" s="10"/>
       <c r="M115" s="6"/>
@@ -6270,7 +6333,7 @@
       </c>
       <c r="E116" s="6"/>
       <c r="F116" s="22" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G116" s="6" t="str">
         <f t="shared" si="6"/>
@@ -6278,13 +6341,13 @@
       </c>
       <c r="H116" s="6"/>
       <c r="I116" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J116" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K116" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L116" s="10"/>
       <c r="M116" s="6"/>
@@ -6310,7 +6373,7 @@
       </c>
       <c r="E117" s="6"/>
       <c r="F117" s="22" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G117" s="6" t="str">
         <f t="shared" si="6"/>
@@ -6321,10 +6384,10 @@
       </c>
       <c r="I117" s="6"/>
       <c r="J117" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K117" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L117" s="10"/>
       <c r="M117" s="6"/>
@@ -6347,7 +6410,7 @@
       </c>
       <c r="E118" s="6"/>
       <c r="F118" s="22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G118" s="6" t="str">
         <f t="shared" si="6"/>
@@ -6358,10 +6421,10 @@
       </c>
       <c r="I118" s="6"/>
       <c r="J118" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K118" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L118" s="10"/>
       <c r="M118" s="6"/>
@@ -6380,25 +6443,25 @@
       </c>
       <c r="C119" s="22"/>
       <c r="D119" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E119" s="22"/>
       <c r="F119" s="22" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G119" s="22" t="str">
         <f t="shared" si="6"/>
         <v>0001110000</v>
       </c>
       <c r="H119" s="22" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="I119" s="22"/>
       <c r="J119" s="22" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="K119" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L119" s="10"/>
       <c r="M119" s="6"/>
@@ -6417,25 +6480,25 @@
       </c>
       <c r="C120" s="22"/>
       <c r="D120" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E120" s="22"/>
       <c r="F120" s="22" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G120" s="22" t="str">
         <f t="shared" si="6"/>
         <v>0001110001</v>
       </c>
       <c r="H120" s="22" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="I120" s="22"/>
       <c r="J120" s="22" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="K120" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L120" s="10"/>
       <c r="M120" s="6"/>
@@ -6454,27 +6517,27 @@
       </c>
       <c r="C121" s="6"/>
       <c r="D121" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E121" s="6"/>
       <c r="F121" s="22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G121" s="6" t="str">
         <f t="shared" si="6"/>
         <v>0001110010</v>
       </c>
       <c r="H121" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I121" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J121" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K121" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L121" s="10"/>
       <c r="M121" s="6"/>
@@ -6493,27 +6556,27 @@
       </c>
       <c r="C122" s="6"/>
       <c r="D122" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E122" s="6"/>
       <c r="F122" s="22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G122" s="6" t="str">
         <f t="shared" si="6"/>
         <v>0001110011</v>
       </c>
       <c r="H122" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I122" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J122" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="K122" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L122" s="10"/>
       <c r="M122" s="6"/>
@@ -6589,11 +6652,11 @@
       </c>
       <c r="C125" s="6"/>
       <c r="D125" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E125" s="6"/>
       <c r="F125" s="22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G125" s="6" t="str">
         <f t="shared" si="6"/>
@@ -6601,13 +6664,13 @@
       </c>
       <c r="H125" s="6"/>
       <c r="I125" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J125" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K125" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L125" s="10"/>
       <c r="M125" s="6"/>
@@ -6626,11 +6689,11 @@
       </c>
       <c r="C126" s="6"/>
       <c r="D126" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E126" s="6"/>
       <c r="F126" s="22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G126" s="6" t="str">
         <f t="shared" si="6"/>
@@ -6638,13 +6701,13 @@
       </c>
       <c r="H126" s="6"/>
       <c r="I126" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J126" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K126" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L126" s="10"/>
       <c r="M126" s="6"/>
@@ -6717,11 +6780,11 @@
       </c>
       <c r="C129" s="6"/>
       <c r="D129" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E129" s="6"/>
       <c r="F129" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G129" s="6" t="str">
         <f t="shared" si="6"/>
@@ -6729,10 +6792,10 @@
       </c>
       <c r="H129" s="6"/>
       <c r="I129" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J129" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K129" s="10"/>
       <c r="L129" s="10"/>
@@ -6765,7 +6828,7 @@
       <c r="I130" s="6"/>
       <c r="J130" s="6"/>
       <c r="K130" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L130" s="10"/>
       <c r="M130" s="6"/>
@@ -6891,14 +6954,14 @@
         <v>128</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D135" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E135" s="6"/>
       <c r="F135" s="22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G135" s="6" t="str">
         <f t="shared" si="6"/>
@@ -6908,26 +6971,26 @@
         <v>16</v>
       </c>
       <c r="I135" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J135" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K135" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L135" s="35" t="s">
+        <v>370</v>
+      </c>
+      <c r="M135" s="35" t="s">
         <v>371</v>
-      </c>
-      <c r="M135" s="35" t="s">
-        <v>372</v>
       </c>
       <c r="N135" s="24"/>
       <c r="O135" s="24">
         <v>2</v>
       </c>
       <c r="P135" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q135" s="7"/>
     </row>
@@ -6940,12 +7003,14 @@
         <v>129</v>
       </c>
       <c r="C136" s="6"/>
-      <c r="D136" s="6"/>
+      <c r="D136" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="E136" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F136" s="22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G136" s="6" t="str">
         <f t="shared" ref="G136:G199" si="10">DEC2BIN(B136, 10)</f>
@@ -6955,26 +7020,26 @@
         <v>16</v>
       </c>
       <c r="I136" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J136" s="22" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K136" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L136" s="35" t="s">
+        <v>370</v>
+      </c>
+      <c r="M136" s="35" t="s">
         <v>371</v>
-      </c>
-      <c r="M136" s="35" t="s">
-        <v>372</v>
       </c>
       <c r="N136" s="24"/>
       <c r="O136" s="24">
         <v>2</v>
       </c>
       <c r="P136" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q136" s="7"/>
     </row>
@@ -6987,12 +7052,14 @@
         <v>130</v>
       </c>
       <c r="C137" s="6"/>
-      <c r="D137" s="6"/>
+      <c r="D137" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="E137" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F137" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G137" s="6" t="str">
         <f t="shared" si="10"/>
@@ -7002,26 +7069,26 @@
         <v>16</v>
       </c>
       <c r="I137" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J137" s="22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K137" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L137" s="35" t="s">
+        <v>370</v>
+      </c>
+      <c r="M137" s="35" t="s">
         <v>371</v>
-      </c>
-      <c r="M137" s="35" t="s">
-        <v>372</v>
       </c>
       <c r="N137" s="24"/>
       <c r="O137" s="24">
         <v>2</v>
       </c>
       <c r="P137" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q137" s="7"/>
     </row>
@@ -7035,11 +7102,11 @@
       </c>
       <c r="C138" s="6"/>
       <c r="D138" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E138" s="6"/>
       <c r="F138" s="22" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G138" s="6" t="str">
         <f t="shared" si="10"/>
@@ -7049,13 +7116,13 @@
         <v>16</v>
       </c>
       <c r="I138" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J138" s="22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K138" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L138" s="6"/>
       <c r="M138" s="6"/>
@@ -7064,7 +7131,7 @@
         <v>2</v>
       </c>
       <c r="P138" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q138" s="7"/>
     </row>
@@ -7077,12 +7144,14 @@
         <v>132</v>
       </c>
       <c r="C139" s="6"/>
-      <c r="D139" s="6"/>
+      <c r="D139" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="E139" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F139" s="22" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G139" s="6" t="str">
         <f t="shared" si="10"/>
@@ -7092,13 +7161,13 @@
         <v>16</v>
       </c>
       <c r="I139" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J139" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K139" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L139" s="6"/>
       <c r="M139" s="6"/>
@@ -7107,7 +7176,7 @@
         <v>2</v>
       </c>
       <c r="P139" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q139" s="7"/>
     </row>
@@ -7120,12 +7189,14 @@
         <v>133</v>
       </c>
       <c r="C140" s="6"/>
-      <c r="D140" s="6"/>
+      <c r="D140" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="E140" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F140" s="22" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G140" s="6" t="str">
         <f t="shared" si="10"/>
@@ -7135,13 +7206,13 @@
         <v>16</v>
       </c>
       <c r="I140" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J140" s="22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K140" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L140" s="6"/>
       <c r="M140" s="6"/>
@@ -7150,7 +7221,7 @@
         <v>2</v>
       </c>
       <c r="P140" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q140" s="7"/>
     </row>
@@ -7218,10 +7289,10 @@
       </c>
       <c r="C143" s="6"/>
       <c r="D143" s="6" t="s">
-        <v>36</v>
+        <v>421</v>
       </c>
       <c r="E143" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F143" s="22" t="s">
         <v>30</v>
@@ -7234,13 +7305,13 @@
         <v>22</v>
       </c>
       <c r="I143" s="35" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="J143" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K143" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L143" s="6"/>
       <c r="M143" s="6"/>
@@ -7249,7 +7320,7 @@
         <v>2</v>
       </c>
       <c r="P143" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q143" s="7"/>
     </row>
@@ -7263,11 +7334,11 @@
       </c>
       <c r="C144" s="6"/>
       <c r="D144" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E144" s="6"/>
       <c r="F144" s="22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G144" s="6" t="str">
         <f t="shared" ref="G144" si="11">DEC2BIN(B144, 10)</f>
@@ -7278,10 +7349,10 @@
       </c>
       <c r="I144" s="6"/>
       <c r="J144" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K144" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L144" s="6"/>
       <c r="M144" s="6"/>
@@ -7290,7 +7361,7 @@
         <v>2</v>
       </c>
       <c r="P144" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q144" s="7"/>
     </row>
@@ -7303,22 +7374,40 @@
         <v>138</v>
       </c>
       <c r="C145" s="6"/>
-      <c r="D145" s="6"/>
+      <c r="D145" s="6" t="s">
+        <v>422</v>
+      </c>
       <c r="E145" s="6"/>
-      <c r="F145" s="22"/>
+      <c r="F145" s="22" t="s">
+        <v>424</v>
+      </c>
       <c r="G145" s="6" t="str">
         <f t="shared" si="10"/>
         <v>0010001010</v>
       </c>
-      <c r="H145" s="6"/>
-      <c r="I145" s="6"/>
-      <c r="J145" s="6"/>
-      <c r="K145" s="6"/>
+      <c r="H145" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="I145" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="J145" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="K145" s="6" t="s">
+        <v>275</v>
+      </c>
       <c r="L145" s="6"/>
       <c r="M145" s="6"/>
-      <c r="N145" s="24"/>
-      <c r="O145" s="24"/>
-      <c r="P145" s="24"/>
+      <c r="N145" s="24" t="s">
+        <v>331</v>
+      </c>
+      <c r="O145" s="24" t="s">
+        <v>433</v>
+      </c>
+      <c r="P145" s="24" t="s">
+        <v>434</v>
+      </c>
       <c r="Q145" s="7"/>
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.15">
@@ -7330,22 +7419,42 @@
         <v>139</v>
       </c>
       <c r="C146" s="6"/>
-      <c r="D146" s="6"/>
-      <c r="E146" s="6"/>
-      <c r="F146" s="22"/>
+      <c r="D146" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="E146" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="F146" s="22" t="s">
+        <v>425</v>
+      </c>
       <c r="G146" s="6" t="str">
         <f t="shared" si="10"/>
         <v>0010001011</v>
       </c>
-      <c r="H146" s="6"/>
-      <c r="I146" s="6"/>
-      <c r="J146" s="6"/>
-      <c r="K146" s="6"/>
+      <c r="H146" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="I146" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="J146" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="K146" s="6" t="s">
+        <v>275</v>
+      </c>
       <c r="L146" s="6"/>
       <c r="M146" s="6"/>
-      <c r="N146" s="24"/>
-      <c r="O146" s="24"/>
-      <c r="P146" s="24"/>
+      <c r="N146" s="24" t="s">
+        <v>331</v>
+      </c>
+      <c r="O146" s="24" t="s">
+        <v>433</v>
+      </c>
+      <c r="P146" s="24" t="s">
+        <v>434</v>
+      </c>
       <c r="Q146" s="7"/>
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.15">
@@ -7357,22 +7466,42 @@
         <v>140</v>
       </c>
       <c r="C147" s="6"/>
-      <c r="D147" s="6"/>
-      <c r="E147" s="6"/>
-      <c r="F147" s="6"/>
+      <c r="D147" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="E147" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="F147" s="6" t="s">
+        <v>426</v>
+      </c>
       <c r="G147" s="6" t="str">
         <f t="shared" si="10"/>
         <v>0010001100</v>
       </c>
-      <c r="H147" s="6"/>
-      <c r="I147" s="6"/>
-      <c r="J147" s="6"/>
-      <c r="K147" s="6"/>
+      <c r="H147" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="I147" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="J147" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="K147" s="6" t="s">
+        <v>275</v>
+      </c>
       <c r="L147" s="6"/>
       <c r="M147" s="6"/>
-      <c r="N147" s="24"/>
-      <c r="O147" s="24"/>
-      <c r="P147" s="24"/>
+      <c r="N147" s="24" t="s">
+        <v>331</v>
+      </c>
+      <c r="O147" s="24" t="s">
+        <v>432</v>
+      </c>
+      <c r="P147" s="24" t="s">
+        <v>434</v>
+      </c>
       <c r="Q147" s="7"/>
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.15">
@@ -7384,22 +7513,40 @@
         <v>141</v>
       </c>
       <c r="C148" s="6"/>
-      <c r="D148" s="6"/>
+      <c r="D148" s="6" t="s">
+        <v>423</v>
+      </c>
       <c r="E148" s="6"/>
-      <c r="F148" s="6"/>
+      <c r="F148" s="6" t="s">
+        <v>427</v>
+      </c>
       <c r="G148" s="6" t="str">
         <f t="shared" ref="G148" si="12">DEC2BIN(B148, 10)</f>
         <v>0010001101</v>
       </c>
-      <c r="H148" s="6"/>
-      <c r="I148" s="6"/>
-      <c r="J148" s="6"/>
-      <c r="K148" s="6"/>
+      <c r="H148" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="I148" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="J148" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="K148" s="6" t="s">
+        <v>275</v>
+      </c>
       <c r="L148" s="6"/>
       <c r="M148" s="6"/>
-      <c r="N148" s="24"/>
-      <c r="O148" s="24"/>
-      <c r="P148" s="24"/>
+      <c r="N148" s="24" t="s">
+        <v>331</v>
+      </c>
+      <c r="O148" s="24" t="s">
+        <v>432</v>
+      </c>
+      <c r="P148" s="24" t="s">
+        <v>434</v>
+      </c>
       <c r="Q148" s="7"/>
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.15">
@@ -7411,22 +7558,42 @@
         <v>142</v>
       </c>
       <c r="C149" s="6"/>
-      <c r="D149" s="6"/>
-      <c r="E149" s="6"/>
-      <c r="F149" s="6"/>
+      <c r="D149" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="E149" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="F149" s="6" t="s">
+        <v>428</v>
+      </c>
       <c r="G149" s="6" t="str">
         <f t="shared" si="10"/>
         <v>0010001110</v>
       </c>
-      <c r="H149" s="6"/>
-      <c r="I149" s="6"/>
-      <c r="J149" s="6"/>
-      <c r="K149" s="6"/>
+      <c r="H149" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="I149" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="J149" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="K149" s="6" t="s">
+        <v>275</v>
+      </c>
       <c r="L149" s="6"/>
       <c r="M149" s="6"/>
-      <c r="N149" s="24"/>
-      <c r="O149" s="24"/>
-      <c r="P149" s="24"/>
+      <c r="N149" s="24" t="s">
+        <v>331</v>
+      </c>
+      <c r="O149" s="24" t="s">
+        <v>432</v>
+      </c>
+      <c r="P149" s="24" t="s">
+        <v>434</v>
+      </c>
       <c r="Q149" s="7"/>
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.15">
@@ -7438,22 +7605,42 @@
         <v>143</v>
       </c>
       <c r="C150" s="6"/>
-      <c r="D150" s="6"/>
-      <c r="E150" s="6"/>
-      <c r="F150" s="6"/>
+      <c r="D150" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="E150" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="F150" s="6" t="s">
+        <v>429</v>
+      </c>
       <c r="G150" s="6" t="str">
         <f t="shared" si="10"/>
         <v>0010001111</v>
       </c>
-      <c r="H150" s="6"/>
-      <c r="I150" s="6"/>
-      <c r="J150" s="6"/>
-      <c r="K150" s="6"/>
+      <c r="H150" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="I150" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="J150" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="K150" s="6" t="s">
+        <v>275</v>
+      </c>
       <c r="L150" s="6"/>
       <c r="M150" s="6"/>
-      <c r="N150" s="24"/>
-      <c r="O150" s="24"/>
-      <c r="P150" s="24"/>
+      <c r="N150" s="24" t="s">
+        <v>331</v>
+      </c>
+      <c r="O150" s="24" t="s">
+        <v>432</v>
+      </c>
+      <c r="P150" s="24" t="s">
+        <v>434</v>
+      </c>
       <c r="Q150" s="7"/>
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.15">
@@ -7481,21 +7668,21 @@
       </c>
       <c r="I151" s="6"/>
       <c r="J151" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K151" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L151" s="6"/>
       <c r="M151" s="35" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="N151" s="24"/>
       <c r="O151" s="24">
         <v>2</v>
       </c>
       <c r="P151" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q151" s="7"/>
     </row>
@@ -7752,30 +7939,30 @@
       </c>
       <c r="C161" s="27"/>
       <c r="D161" s="27" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E161" s="27" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F161" s="28" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G161" s="27" t="str">
         <f t="shared" si="10"/>
         <v>0010011010</v>
       </c>
       <c r="H161" s="27" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I161" s="27"/>
       <c r="J161" s="22" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="K161" s="22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L161" s="22" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="M161" s="22"/>
       <c r="N161" s="30"/>
@@ -7783,7 +7970,7 @@
         <v>2</v>
       </c>
       <c r="P161" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q161" s="45"/>
     </row>
@@ -7797,30 +7984,30 @@
       </c>
       <c r="C162" s="27"/>
       <c r="D162" s="27" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E162" s="27" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F162" s="28" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G162" s="27" t="str">
         <f t="shared" si="10"/>
         <v>0010011011</v>
       </c>
       <c r="H162" s="27" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I162" s="27"/>
       <c r="J162" s="22" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="K162" s="22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L162" s="22" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="M162" s="22"/>
       <c r="N162" s="30"/>
@@ -7828,7 +8015,7 @@
         <v>2</v>
       </c>
       <c r="P162" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q162" s="45"/>
     </row>
@@ -7842,30 +8029,30 @@
       </c>
       <c r="C163" s="27"/>
       <c r="D163" s="27" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E163" s="27" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F163" s="28" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G163" s="27" t="str">
         <f t="shared" si="10"/>
         <v>0010011100</v>
       </c>
       <c r="H163" s="27" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I163" s="27"/>
       <c r="J163" s="22" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="K163" s="22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L163" s="22" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M163" s="22"/>
       <c r="N163" s="30"/>
@@ -7873,7 +8060,7 @@
         <v>2</v>
       </c>
       <c r="P163" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q163" s="45"/>
     </row>
@@ -7887,27 +8074,27 @@
       </c>
       <c r="C164" s="27"/>
       <c r="D164" s="27" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E164" s="27" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F164" s="28" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G164" s="27" t="str">
         <f t="shared" si="10"/>
         <v>0010011101</v>
       </c>
       <c r="H164" s="27" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I164" s="27"/>
       <c r="J164" s="22" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="K164" s="22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L164" s="22"/>
       <c r="M164" s="22"/>
@@ -7916,7 +8103,7 @@
         <v>2</v>
       </c>
       <c r="P164" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q164" s="45"/>
     </row>
@@ -7930,27 +8117,27 @@
       </c>
       <c r="C165" s="27"/>
       <c r="D165" s="27" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E165" s="27" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F165" s="28" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G165" s="27" t="str">
         <f t="shared" si="10"/>
         <v>0010011110</v>
       </c>
       <c r="H165" s="27" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I165" s="27"/>
       <c r="J165" s="22" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K165" s="22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L165" s="22"/>
       <c r="M165" s="22"/>
@@ -7959,7 +8146,7 @@
         <v>2</v>
       </c>
       <c r="P165" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q165" s="45"/>
     </row>
@@ -7973,27 +8160,27 @@
       </c>
       <c r="C166" s="27"/>
       <c r="D166" s="27" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E166" s="27" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F166" s="28" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G166" s="27" t="str">
         <f t="shared" si="10"/>
         <v>0010011111</v>
       </c>
       <c r="H166" s="27" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I166" s="27"/>
       <c r="J166" s="22" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K166" s="22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L166" s="22"/>
       <c r="M166" s="22"/>
@@ -8002,7 +8189,7 @@
         <v>2</v>
       </c>
       <c r="P166" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q166" s="45"/>
     </row>
@@ -8015,32 +8202,32 @@
         <v>160</v>
       </c>
       <c r="C167" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D167" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E167" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F167" s="28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G167" s="6" t="str">
         <f t="shared" si="10"/>
         <v>0010100000</v>
       </c>
       <c r="H167" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I167" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J167" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K167" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L167" s="6"/>
       <c r="M167" s="6"/>
@@ -8049,10 +8236,10 @@
         <v>2</v>
       </c>
       <c r="P167" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q167" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="168" spans="1:17" x14ac:dyDescent="0.15">
@@ -8065,29 +8252,29 @@
       </c>
       <c r="C168" s="6"/>
       <c r="D168" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E168" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F168" s="22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G168" s="6" t="str">
         <f t="shared" si="10"/>
         <v>0010100001</v>
       </c>
       <c r="H168" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I168" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J168" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K168" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L168" s="6"/>
       <c r="M168" s="6"/>
@@ -8096,10 +8283,10 @@
         <v>2</v>
       </c>
       <c r="P168" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q168" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="169" spans="1:17" x14ac:dyDescent="0.15">
@@ -8112,29 +8299,29 @@
       </c>
       <c r="C169" s="6"/>
       <c r="D169" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E169" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F169" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G169" s="6" t="str">
         <f t="shared" si="10"/>
         <v>0010100010</v>
       </c>
       <c r="H169" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I169" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J169" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K169" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L169" s="6"/>
       <c r="M169" s="6"/>
@@ -8143,10 +8330,10 @@
         <v>2</v>
       </c>
       <c r="P169" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q169" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="170" spans="1:17" x14ac:dyDescent="0.15">
@@ -8159,27 +8346,27 @@
       </c>
       <c r="C170" s="6"/>
       <c r="D170" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E170" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F170" s="22" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G170" s="6" t="str">
         <f t="shared" si="10"/>
         <v>0010100011</v>
       </c>
       <c r="H170" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I170" s="9"/>
       <c r="J170" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K170" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L170" s="6"/>
       <c r="M170" s="6"/>
@@ -8188,10 +8375,10 @@
         <v>2</v>
       </c>
       <c r="P170" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q170" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="171" spans="1:17" x14ac:dyDescent="0.15">
@@ -8528,29 +8715,29 @@
       </c>
       <c r="C183" s="6"/>
       <c r="D183" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E183" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F183" s="28" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G183" s="6" t="str">
         <f t="shared" si="10"/>
         <v>0010110000</v>
       </c>
       <c r="H183" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I183" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J183" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K183" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L183" s="6"/>
       <c r="M183" s="6"/>
@@ -8559,10 +8746,10 @@
         <v>2</v>
       </c>
       <c r="P183" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q183" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="184" spans="1:17" x14ac:dyDescent="0.15">
@@ -8575,29 +8762,29 @@
       </c>
       <c r="C184" s="6"/>
       <c r="D184" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E184" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F184" s="22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G184" s="6" t="str">
         <f t="shared" si="10"/>
         <v>0010110001</v>
       </c>
       <c r="H184" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I184" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J184" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K184" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L184" s="6"/>
       <c r="M184" s="6"/>
@@ -8606,10 +8793,10 @@
         <v>2</v>
       </c>
       <c r="P184" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q184" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="185" spans="1:17" x14ac:dyDescent="0.15">
@@ -8622,29 +8809,29 @@
       </c>
       <c r="C185" s="6"/>
       <c r="D185" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E185" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F185" s="22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G185" s="6" t="str">
         <f t="shared" si="10"/>
         <v>0010110010</v>
       </c>
       <c r="H185" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I185" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J185" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K185" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L185" s="6"/>
       <c r="M185" s="6"/>
@@ -8653,10 +8840,10 @@
         <v>2</v>
       </c>
       <c r="P185" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q185" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="186" spans="1:17" x14ac:dyDescent="0.15">
@@ -9019,14 +9206,14 @@
         <v>192</v>
       </c>
       <c r="C199" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D199" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E199" s="6"/>
       <c r="F199" s="22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G199" s="6" t="str">
         <f t="shared" si="10"/>
@@ -9037,10 +9224,10 @@
       </c>
       <c r="I199" s="6"/>
       <c r="J199" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K199" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L199" s="6"/>
       <c r="M199" s="22"/>
@@ -9059,11 +9246,11 @@
       </c>
       <c r="C200" s="6"/>
       <c r="D200" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E200" s="6"/>
       <c r="F200" s="22" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G200" s="6" t="str">
         <f t="shared" ref="G200:G201" si="15">DEC2BIN(B200, 10)</f>
@@ -9074,10 +9261,10 @@
       </c>
       <c r="I200" s="6"/>
       <c r="J200" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K200" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L200" s="6"/>
       <c r="M200" s="10"/>
@@ -9096,11 +9283,11 @@
       </c>
       <c r="C201" s="6"/>
       <c r="D201" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E201" s="6"/>
       <c r="F201" s="22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G201" s="6" t="str">
         <f t="shared" si="15"/>
@@ -9111,10 +9298,10 @@
       </c>
       <c r="I201" s="6"/>
       <c r="J201" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K201" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L201" s="6"/>
       <c r="M201" s="6"/>
@@ -9133,11 +9320,11 @@
       </c>
       <c r="C202" s="6"/>
       <c r="D202" s="22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E202" s="22"/>
       <c r="F202" s="22" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G202" s="6" t="str">
         <f t="shared" ref="G202:G208" si="16">DEC2BIN(B202, 10)</f>
@@ -9148,10 +9335,10 @@
       </c>
       <c r="I202" s="6"/>
       <c r="J202" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K202" s="35" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L202" s="35"/>
       <c r="M202" s="10"/>
@@ -9170,11 +9357,11 @@
       </c>
       <c r="C203" s="6"/>
       <c r="D203" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E203" s="6"/>
       <c r="F203" s="22" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G203" s="6" t="str">
         <f t="shared" si="16"/>
@@ -9185,10 +9372,10 @@
       </c>
       <c r="I203" s="6"/>
       <c r="J203" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K203" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L203" s="6"/>
       <c r="M203" s="6"/>
@@ -9207,11 +9394,11 @@
       </c>
       <c r="C204" s="6"/>
       <c r="D204" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E204" s="22"/>
       <c r="F204" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G204" s="6" t="str">
         <f t="shared" si="16"/>
@@ -9222,10 +9409,10 @@
       </c>
       <c r="I204" s="6"/>
       <c r="J204" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K204" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L204" s="6"/>
       <c r="M204" s="6"/>
@@ -9233,7 +9420,7 @@
       <c r="O204" s="24"/>
       <c r="P204" s="24"/>
       <c r="Q204" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="205" spans="1:17" x14ac:dyDescent="0.15">
@@ -9300,36 +9487,36 @@
       </c>
       <c r="C207" s="6"/>
       <c r="D207" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E207" s="6"/>
       <c r="F207" s="22" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G207" s="6" t="str">
         <f t="shared" si="16"/>
         <v>0011001000</v>
       </c>
       <c r="H207" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I207" s="6"/>
       <c r="J207" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K207" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L207" s="6"/>
       <c r="M207" s="10"/>
       <c r="N207" s="24" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="O207" s="24">
         <v>3</v>
       </c>
       <c r="P207" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q207" s="7"/>
     </row>
@@ -9343,36 +9530,36 @@
       </c>
       <c r="C208" s="6"/>
       <c r="D208" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E208" s="6"/>
       <c r="F208" s="22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G208" s="6" t="str">
         <f t="shared" si="16"/>
         <v>0011001001</v>
       </c>
       <c r="H208" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I208" s="6"/>
       <c r="J208" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K208" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L208" s="6"/>
       <c r="M208" s="6"/>
       <c r="N208" s="24" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="O208" s="24">
         <v>3</v>
       </c>
       <c r="P208" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q208" s="7"/>
     </row>
@@ -9386,25 +9573,25 @@
       </c>
       <c r="C209" s="6"/>
       <c r="D209" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E209" s="6"/>
       <c r="F209" s="22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G209" s="6" t="str">
         <f t="shared" ref="G209:G262" si="17">DEC2BIN(B209, 10)</f>
         <v>0011001010</v>
       </c>
       <c r="H209" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I209" s="6"/>
       <c r="J209" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K209" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L209" s="6"/>
       <c r="M209" s="6"/>
@@ -9412,7 +9599,7 @@
       <c r="O209" s="24"/>
       <c r="P209" s="24"/>
       <c r="Q209" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="210" spans="1:17" x14ac:dyDescent="0.15">
@@ -9425,25 +9612,25 @@
       </c>
       <c r="C210" s="6"/>
       <c r="D210" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E210" s="6"/>
       <c r="F210" s="22" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G210" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011001011</v>
       </c>
       <c r="H210" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I210" s="6"/>
       <c r="J210" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K210" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L210" s="6"/>
       <c r="M210" s="6"/>
@@ -9462,25 +9649,25 @@
       </c>
       <c r="C211" s="6"/>
       <c r="D211" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E211" s="6"/>
       <c r="F211" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G211" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011001100</v>
       </c>
       <c r="H211" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I211" s="6"/>
       <c r="J211" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K211" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L211" s="6"/>
       <c r="M211" s="6"/>
@@ -9499,23 +9686,23 @@
       </c>
       <c r="C212" s="6"/>
       <c r="D212" s="34" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E212" s="34"/>
       <c r="F212" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G212" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011001101</v>
       </c>
       <c r="H212" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I212" s="6"/>
       <c r="J212" s="6"/>
       <c r="K212" s="35" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L212" s="35"/>
       <c r="M212" s="6"/>
@@ -9534,23 +9721,23 @@
       </c>
       <c r="C213" s="6"/>
       <c r="D213" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E213" s="6"/>
       <c r="F213" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G213" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011001110</v>
       </c>
       <c r="H213" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I213" s="6"/>
       <c r="J213" s="6"/>
       <c r="K213" s="35" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L213" s="35"/>
       <c r="M213" s="6"/>
@@ -9576,7 +9763,7 @@
         <v>0011001111</v>
       </c>
       <c r="H214" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I214" s="6"/>
       <c r="J214" s="6"/>
@@ -9598,23 +9785,23 @@
       </c>
       <c r="C215" s="6"/>
       <c r="D215" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E215" s="6"/>
       <c r="F215" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G215" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011010000</v>
       </c>
       <c r="H215" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I215" s="6"/>
       <c r="J215" s="6"/>
       <c r="K215" s="35" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L215" s="35"/>
       <c r="M215" s="6"/>
@@ -9633,23 +9820,23 @@
       </c>
       <c r="C216" s="6"/>
       <c r="D216" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E216" s="6"/>
       <c r="F216" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G216" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011010001</v>
       </c>
       <c r="H216" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I216" s="6"/>
       <c r="J216" s="6"/>
       <c r="K216" s="35" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L216" s="35"/>
       <c r="M216" s="6"/>
@@ -9695,23 +9882,23 @@
       </c>
       <c r="C218" s="22"/>
       <c r="D218" s="22" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E218" s="22"/>
       <c r="F218" s="22" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G218" s="22" t="str">
         <f t="shared" si="17"/>
         <v>0011010011</v>
       </c>
       <c r="H218" s="22" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I218" s="22"/>
       <c r="J218" s="22"/>
       <c r="K218" s="22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L218" s="22"/>
       <c r="M218" s="6"/>
@@ -9730,23 +9917,23 @@
       </c>
       <c r="C219" s="22"/>
       <c r="D219" s="22" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E219" s="22"/>
       <c r="F219" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G219" s="22" t="str">
         <f t="shared" si="17"/>
         <v>0011010100</v>
       </c>
       <c r="H219" s="22" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I219" s="22"/>
       <c r="J219" s="22"/>
       <c r="K219" s="22" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="L219" s="22"/>
       <c r="M219" s="6"/>
@@ -9765,23 +9952,23 @@
       </c>
       <c r="C220" s="22"/>
       <c r="D220" s="22" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E220" s="22"/>
       <c r="F220" s="22" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G220" s="22" t="str">
         <f t="shared" si="17"/>
         <v>0011010101</v>
       </c>
       <c r="H220" s="22" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I220" s="22"/>
       <c r="J220" s="22"/>
       <c r="K220" s="22" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="L220" s="22"/>
       <c r="M220" s="6"/>
@@ -9800,23 +9987,23 @@
       </c>
       <c r="C221" s="22"/>
       <c r="D221" s="22" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E221" s="22"/>
       <c r="F221" s="22" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G221" s="22" t="str">
         <f t="shared" si="17"/>
         <v>0011010110</v>
       </c>
       <c r="H221" s="22" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I221" s="22"/>
       <c r="J221" s="22"/>
       <c r="K221" s="22" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="L221" s="22"/>
       <c r="M221" s="6"/>
@@ -9835,25 +10022,25 @@
       </c>
       <c r="C222" s="32"/>
       <c r="D222" s="32" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E222" s="32"/>
       <c r="F222" s="32" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G222" s="32" t="str">
         <f t="shared" si="17"/>
         <v>0011010111</v>
       </c>
       <c r="H222" s="32" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="I222" s="32"/>
       <c r="J222" s="32" t="s">
+        <v>329</v>
+      </c>
+      <c r="K222" s="32" t="s">
         <v>330</v>
-      </c>
-      <c r="K222" s="32" t="s">
-        <v>331</v>
       </c>
       <c r="L222" s="32"/>
       <c r="M222" s="6"/>
@@ -9872,25 +10059,25 @@
       </c>
       <c r="C223" s="6"/>
       <c r="D223" s="6" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E223" s="6"/>
       <c r="F223" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G223" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011011000</v>
       </c>
       <c r="H223" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="I223" s="6"/>
       <c r="J223" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="K223" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="L223" s="6"/>
       <c r="M223" s="6"/>
@@ -9909,25 +10096,25 @@
       </c>
       <c r="C224" s="6"/>
       <c r="D224" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E224" s="6"/>
       <c r="F224" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G224" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011011001</v>
       </c>
       <c r="H224" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="I224" s="6"/>
       <c r="J224" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="K224" s="6" t="s">
         <v>412</v>
-      </c>
-      <c r="K224" s="6" t="s">
-        <v>413</v>
       </c>
       <c r="L224" s="6"/>
       <c r="M224" s="6"/>
@@ -10107,14 +10294,14 @@
         <v>224</v>
       </c>
       <c r="C231" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D231" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E231" s="6"/>
       <c r="F231" s="22" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G231" s="6" t="str">
         <f t="shared" si="17"/>
@@ -10125,10 +10312,10 @@
       </c>
       <c r="I231" s="6"/>
       <c r="J231" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K231" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L231" s="6"/>
       <c r="M231" s="6"/>
@@ -10147,11 +10334,11 @@
       </c>
       <c r="C232" s="32"/>
       <c r="D232" s="32" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E232" s="32"/>
       <c r="F232" s="32" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G232" s="32" t="str">
         <f t="shared" si="17"/>
@@ -10163,16 +10350,16 @@
       <c r="I232" s="32"/>
       <c r="J232" s="32"/>
       <c r="K232" s="32" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L232" s="32"/>
       <c r="M232" s="6"/>
       <c r="N232" s="24" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="O232" s="24"/>
       <c r="P232" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q232" s="7"/>
     </row>
@@ -10196,7 +10383,7 @@
       <c r="I233" s="6"/>
       <c r="J233" s="6"/>
       <c r="K233" s="22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L233" s="22"/>
       <c r="M233" s="6"/>
@@ -10269,41 +10456,41 @@
       </c>
       <c r="C236" s="6"/>
       <c r="D236" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E236" s="22"/>
       <c r="F236" s="22" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G236" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011100101</v>
       </c>
       <c r="H236" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I236" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J236" s="6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K236" s="22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L236" s="22"/>
       <c r="M236" s="6"/>
       <c r="N236" s="24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O236" s="24">
         <v>3</v>
       </c>
       <c r="P236" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q236" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="Q236" s="7" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="237" spans="1:17" x14ac:dyDescent="0.15">
@@ -10370,36 +10557,36 @@
       </c>
       <c r="C239" s="6"/>
       <c r="D239" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E239" s="6"/>
       <c r="F239" s="22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G239" s="6" t="str">
         <f>DEC2BIN(B239, 10)</f>
         <v>0011101000</v>
       </c>
       <c r="H239" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I239" s="6"/>
       <c r="J239" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K239" s="22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L239" s="22"/>
       <c r="M239" s="6"/>
       <c r="N239" s="24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O239" s="24">
         <v>3</v>
       </c>
       <c r="P239" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q239" s="7"/>
     </row>
@@ -10413,36 +10600,36 @@
       </c>
       <c r="C240" s="6"/>
       <c r="D240" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E240" s="6"/>
       <c r="F240" s="22" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G240" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011101001</v>
       </c>
       <c r="H240" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I240" s="6"/>
       <c r="J240" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K240" s="22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L240" s="22"/>
       <c r="M240" s="6"/>
       <c r="N240" s="24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O240" s="24">
         <v>3</v>
       </c>
       <c r="P240" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q240" s="7"/>
     </row>
@@ -10456,41 +10643,41 @@
       </c>
       <c r="C241" s="6"/>
       <c r="D241" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E241" s="6"/>
       <c r="F241" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G241" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011101010</v>
       </c>
       <c r="H241" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I241" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J241" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="K241" s="22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L241" s="22"/>
       <c r="M241" s="6"/>
       <c r="N241" s="24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O241" s="24">
         <v>3</v>
       </c>
       <c r="P241" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q241" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="242" spans="1:17" x14ac:dyDescent="0.15">
@@ -10557,23 +10744,23 @@
       </c>
       <c r="C244" s="6"/>
       <c r="D244" s="34" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E244" s="34"/>
       <c r="F244" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G244" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011101101</v>
       </c>
       <c r="H244" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I244" s="6"/>
       <c r="J244" s="6"/>
       <c r="K244" s="22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L244" s="22"/>
       <c r="M244" s="6"/>
@@ -10592,23 +10779,23 @@
       </c>
       <c r="C245" s="6"/>
       <c r="D245" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E245" s="6"/>
       <c r="F245" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G245" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011101110</v>
       </c>
       <c r="H245" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I245" s="6"/>
       <c r="J245" s="6"/>
       <c r="K245" s="22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L245" s="22"/>
       <c r="M245" s="6"/>
@@ -10634,7 +10821,7 @@
         <v>0011101111</v>
       </c>
       <c r="H246" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I246" s="22"/>
       <c r="J246" s="22"/>
@@ -10656,23 +10843,23 @@
       </c>
       <c r="C247" s="22"/>
       <c r="D247" s="22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E247" s="22"/>
       <c r="F247" s="22" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G247" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011110000</v>
       </c>
       <c r="H247" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I247" s="6"/>
       <c r="J247" s="6"/>
       <c r="K247" s="22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L247" s="22"/>
       <c r="M247" s="6"/>
@@ -10691,23 +10878,23 @@
       </c>
       <c r="C248" s="22"/>
       <c r="D248" s="22" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E248" s="22"/>
       <c r="F248" s="22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G248" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011110001</v>
       </c>
       <c r="H248" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I248" s="6"/>
       <c r="J248" s="6"/>
       <c r="K248" s="22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L248" s="22"/>
       <c r="M248" s="6"/>
@@ -10726,23 +10913,23 @@
       </c>
       <c r="C249" s="22"/>
       <c r="D249" s="22" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E249" s="22"/>
       <c r="F249" s="22" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G249" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011110010</v>
       </c>
       <c r="H249" s="6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I249" s="6"/>
       <c r="J249" s="6"/>
       <c r="K249" s="22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L249" s="22"/>
       <c r="M249" s="6"/>
@@ -10761,23 +10948,23 @@
       </c>
       <c r="C250" s="22"/>
       <c r="D250" s="22" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E250" s="22"/>
       <c r="F250" s="22" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G250" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011110011</v>
       </c>
       <c r="H250" s="6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I250" s="6"/>
       <c r="J250" s="6"/>
       <c r="K250" s="22" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="L250" s="22"/>
       <c r="M250" s="6"/>
@@ -10796,23 +10983,23 @@
       </c>
       <c r="C251" s="22"/>
       <c r="D251" s="22" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E251" s="22"/>
       <c r="F251" s="22" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G251" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011110100</v>
       </c>
       <c r="H251" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I251" s="6"/>
       <c r="J251" s="6"/>
       <c r="K251" s="22" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="L251" s="22"/>
       <c r="M251" s="6"/>
@@ -10831,23 +11018,23 @@
       </c>
       <c r="C252" s="22"/>
       <c r="D252" s="22" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E252" s="22"/>
       <c r="F252" s="22" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G252" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011110101</v>
       </c>
       <c r="H252" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I252" s="6"/>
       <c r="J252" s="6"/>
       <c r="K252" s="22" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="L252" s="22"/>
       <c r="M252" s="6"/>
@@ -10866,23 +11053,23 @@
       </c>
       <c r="C253" s="22"/>
       <c r="D253" s="22" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E253" s="22"/>
       <c r="F253" s="22" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G253" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011110110</v>
       </c>
       <c r="H253" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I253" s="6"/>
       <c r="J253" s="6"/>
       <c r="K253" s="22" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="L253" s="22"/>
       <c r="M253" s="6"/>
@@ -11117,13 +11304,13 @@
       </c>
       <c r="C262" s="35"/>
       <c r="D262" s="35" t="s">
+        <v>381</v>
+      </c>
+      <c r="E262" s="35" t="s">
+        <v>277</v>
+      </c>
+      <c r="F262" s="35" t="s">
         <v>382</v>
-      </c>
-      <c r="E262" s="35" t="s">
-        <v>278</v>
-      </c>
-      <c r="F262" s="35" t="s">
-        <v>383</v>
       </c>
       <c r="G262" s="35" t="str">
         <f t="shared" si="17"/>
@@ -11131,13 +11318,13 @@
       </c>
       <c r="H262" s="35"/>
       <c r="I262" s="35" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="J262" s="6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="K262" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L262" s="6"/>
       <c r="M262" s="6"/>
@@ -11173,10 +11360,10 @@
       </c>
       <c r="I263" s="6"/>
       <c r="J263" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K263" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L263" s="6"/>
       <c r="M263" s="6"/>
@@ -11195,7 +11382,7 @@
       </c>
       <c r="C264" s="6"/>
       <c r="D264" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E264" s="6"/>
       <c r="F264" s="6" t="s">
@@ -11210,21 +11397,21 @@
       </c>
       <c r="I264" s="6"/>
       <c r="J264" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K264" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L264" s="6"/>
       <c r="M264" s="6"/>
       <c r="N264" s="24" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="O264" s="24">
         <v>3</v>
       </c>
       <c r="P264" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q264" s="7"/>
     </row>
@@ -11253,10 +11440,10 @@
       </c>
       <c r="I265" s="6"/>
       <c r="J265" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K265" s="35" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L265" s="35"/>
       <c r="M265" s="6"/>
@@ -11275,29 +11462,29 @@
       </c>
       <c r="C266" s="6"/>
       <c r="D266" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E266" s="22" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F266" s="22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G266" s="6" t="str">
         <f t="shared" ref="G266:G327" si="20">DEC2BIN(B266, 10)</f>
         <v>0100000011</v>
       </c>
       <c r="H266" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I266" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J266" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K266" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L266" s="6"/>
       <c r="M266" s="6"/>
@@ -12071,14 +12258,14 @@
         <v>288</v>
       </c>
       <c r="C295" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D295" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E295" s="6"/>
       <c r="F295" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G295" s="6" t="str">
         <f t="shared" si="20"/>
@@ -12086,13 +12273,13 @@
       </c>
       <c r="H295" s="6"/>
       <c r="I295" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="J295" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="J295" s="6" t="s">
-        <v>218</v>
-      </c>
       <c r="K295" s="35" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L295" s="35"/>
       <c r="M295" s="6"/>
@@ -12111,27 +12298,27 @@
       </c>
       <c r="C296" s="6"/>
       <c r="D296" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E296" s="6"/>
       <c r="F296" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G296" s="6" t="str">
         <f t="shared" si="20"/>
         <v>0100100001</v>
       </c>
       <c r="H296" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="I296" s="6" t="s">
         <v>394</v>
       </c>
-      <c r="I296" s="6" t="s">
+      <c r="J296" s="6" t="s">
         <v>395</v>
       </c>
-      <c r="J296" s="6" t="s">
-        <v>396</v>
-      </c>
       <c r="K296" s="35" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L296" s="35"/>
       <c r="M296" s="6"/>
@@ -12150,37 +12337,37 @@
       </c>
       <c r="C297" s="6"/>
       <c r="D297" s="27" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E297" s="28"/>
       <c r="F297" s="28" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G297" s="28" t="str">
         <f t="shared" si="20"/>
         <v>0100100010</v>
       </c>
       <c r="H297" s="28" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I297" s="28"/>
       <c r="J297" s="28" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K297" s="28" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L297" s="28"/>
       <c r="M297" s="28"/>
       <c r="N297" s="39" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O297" s="39"/>
       <c r="P297" s="39" t="s">
+        <v>287</v>
+      </c>
+      <c r="Q297" s="40" t="s">
         <v>288</v>
-      </c>
-      <c r="Q297" s="40" t="s">
-        <v>289</v>
       </c>
       <c r="R297" s="41"/>
     </row>
@@ -12194,11 +12381,11 @@
       </c>
       <c r="C298" s="6"/>
       <c r="D298" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E298" s="6"/>
       <c r="F298" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G298" s="6" t="str">
         <f t="shared" si="20"/>
@@ -12225,11 +12412,11 @@
       </c>
       <c r="C299" s="6"/>
       <c r="D299" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E299" s="6"/>
       <c r="F299" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G299" s="6" t="str">
         <f t="shared" si="20"/>

</xml_diff>

<commit_message>
Add instructions : Type-E(SRPPCR, SRPPSR)
</commit_message>
<xml_diff>
--- a/instructions/mist32_isa.xlsx
+++ b/instructions/mist32_isa.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="438">
   <si>
     <t>ADD</t>
     <phoneticPr fontId="1"/>
@@ -2910,8 +2910,8 @@
   </sheetPr>
   <dimension ref="A2:AL1031"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A250" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F271" sqref="F271"/>
+    <sheetView tabSelected="1" topLeftCell="A226" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C213" sqref="C213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -10097,7 +10097,9 @@
       <c r="B212" s="6">
         <v>205</v>
       </c>
-      <c r="C212" s="24"/>
+      <c r="C212" s="24" t="s">
+        <v>436</v>
+      </c>
       <c r="D212" s="6"/>
       <c r="E212" s="34" t="s">
         <v>253</v>
@@ -10133,7 +10135,9 @@
       <c r="B213" s="6">
         <v>206</v>
       </c>
-      <c r="C213" s="24"/>
+      <c r="C213" s="24" t="s">
+        <v>436</v>
+      </c>
       <c r="D213" s="6"/>
       <c r="E213" s="6" t="s">
         <v>250</v>

</xml_diff>

<commit_message>
Add instructions for Type-E : SRFRCLR, SRFRCHR, IDTS
</commit_message>
<xml_diff>
--- a/instructions/mist32_isa.xlsx
+++ b/instructions/mist32_isa.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="438">
   <si>
     <t>ADD</t>
     <phoneticPr fontId="1"/>
@@ -1477,10 +1477,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>FRCR -&gt; {FRCHR, FRCLW}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>FRCHR Read</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -2057,6 +2053,10 @@
   </si>
   <si>
     <t>SRSPADD</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FRCR -&gt; {FRCHR, FRCLR}</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2910,8 +2910,8 @@
   </sheetPr>
   <dimension ref="A2:AL1031"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A226" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C213" sqref="C213"/>
+    <sheetView tabSelected="1" topLeftCell="A274" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C297" sqref="C297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2964,58 +2964,58 @@
     </row>
     <row r="6" spans="1:20" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
+        <v>386</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>387</v>
       </c>
-      <c r="B6" s="18" t="s">
-        <v>388</v>
-      </c>
       <c r="C6" s="18" t="s">
+        <v>432</v>
+      </c>
+      <c r="D6" s="18" t="s">
         <v>433</v>
       </c>
-      <c r="D6" s="18" t="s">
-        <v>434</v>
-      </c>
       <c r="E6" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>413</v>
+      </c>
+      <c r="G6" s="18" t="s">
         <v>364</v>
       </c>
-      <c r="F6" s="18" t="s">
-        <v>414</v>
-      </c>
-      <c r="G6" s="18" t="s">
+      <c r="H6" s="18" t="s">
         <v>365</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="I6" s="18" t="s">
+        <v>396</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>397</v>
+      </c>
+      <c r="K6" s="18" t="s">
         <v>366</v>
       </c>
-      <c r="I6" s="18" t="s">
-        <v>397</v>
-      </c>
-      <c r="J6" s="18" t="s">
+      <c r="L6" s="18" t="s">
+        <v>389</v>
+      </c>
+      <c r="M6" s="29" t="s">
         <v>398</v>
       </c>
-      <c r="K6" s="18" t="s">
-        <v>367</v>
-      </c>
-      <c r="L6" s="18" t="s">
-        <v>390</v>
-      </c>
-      <c r="M6" s="29" t="s">
+      <c r="N6" s="43" t="s">
         <v>399</v>
       </c>
-      <c r="N6" s="43" t="s">
+      <c r="O6" s="26" t="s">
         <v>400</v>
       </c>
-      <c r="O6" s="26" t="s">
+      <c r="P6" s="33" t="s">
         <v>401</v>
       </c>
-      <c r="P6" s="33" t="s">
+      <c r="Q6" s="33" t="s">
         <v>402</v>
       </c>
-      <c r="Q6" s="33" t="s">
+      <c r="R6" s="19" t="s">
         <v>403</v>
-      </c>
-      <c r="R6" s="19" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
@@ -3027,7 +3027,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>44</v>
@@ -3071,7 +3071,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6" t="s">
@@ -3113,7 +3113,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6" t="s">
@@ -3136,7 +3136,7 @@
         <v>143</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
@@ -3155,7 +3155,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6" t="s">
@@ -3178,7 +3178,7 @@
         <v>143</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
@@ -3281,7 +3281,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="22" t="s">
@@ -3426,11 +3426,11 @@
         <v>0000001001</v>
       </c>
       <c r="I16" s="22" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="J16" s="22"/>
       <c r="K16" s="22" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="L16" s="22" t="s">
         <v>275</v>
@@ -3453,25 +3453,25 @@
         <v>10</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D17" s="35"/>
       <c r="E17" s="35" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F17" s="35"/>
       <c r="G17" s="35" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="H17" s="35" t="str">
         <f t="shared" si="2"/>
         <v>0000001010</v>
       </c>
       <c r="I17" s="35" t="s">
+        <v>383</v>
+      </c>
+      <c r="J17" s="35" t="s">
         <v>384</v>
-      </c>
-      <c r="J17" s="35" t="s">
-        <v>385</v>
       </c>
       <c r="K17" s="35"/>
       <c r="L17" s="35"/>
@@ -3493,25 +3493,25 @@
         <v>11</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D18" s="35"/>
       <c r="E18" s="35" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F18" s="35"/>
       <c r="G18" s="35" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H18" s="35" t="str">
         <f t="shared" si="2"/>
         <v>0000001011</v>
       </c>
       <c r="I18" s="35" t="s">
+        <v>383</v>
+      </c>
+      <c r="J18" s="35" t="s">
         <v>384</v>
-      </c>
-      <c r="J18" s="35" t="s">
-        <v>385</v>
       </c>
       <c r="K18" s="35"/>
       <c r="L18" s="35"/>
@@ -3565,22 +3565,22 @@
       <c r="C20" s="24"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F20" s="22"/>
       <c r="G20" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="H20" s="6" t="str">
         <f t="shared" si="2"/>
         <v>0000001101</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J20" s="6"/>
       <c r="K20" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
@@ -3599,7 +3599,7 @@
         <v>14</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6" t="s">
@@ -3669,7 +3669,7 @@
         <v>16</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6" t="s">
@@ -3707,7 +3707,7 @@
         <v>17</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6" t="s">
@@ -3775,27 +3775,27 @@
       <c r="C26" s="24"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="H26" s="6" t="str">
         <f t="shared" si="2"/>
         <v>0000010011</v>
       </c>
       <c r="I26" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="J26" s="6" t="s">
         <v>340</v>
       </c>
-      <c r="J26" s="6" t="s">
+      <c r="K26" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="K26" s="6" t="s">
-        <v>342</v>
-      </c>
       <c r="L26" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M26" s="6"/>
       <c r="N26" s="6"/>
@@ -3815,27 +3815,27 @@
       <c r="C27" s="24"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H27" s="6" t="str">
         <f t="shared" si="2"/>
         <v>0000010100</v>
       </c>
       <c r="I27" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="J27" s="6" t="s">
         <v>340</v>
       </c>
-      <c r="J27" s="6" t="s">
-        <v>341</v>
-      </c>
       <c r="K27" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="L27" s="6" t="s">
         <v>343</v>
-      </c>
-      <c r="L27" s="6" t="s">
-        <v>344</v>
       </c>
       <c r="M27" s="6"/>
       <c r="N27" s="6"/>
@@ -3855,27 +3855,27 @@
       <c r="C28" s="24"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H28" s="6" t="str">
         <f>DEC2BIN(B28, 10)</f>
         <v>0000010101</v>
       </c>
       <c r="I28" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="J28" s="6" t="s">
         <v>340</v>
       </c>
-      <c r="J28" s="6" t="s">
+      <c r="K28" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="K28" s="6" t="s">
-        <v>342</v>
-      </c>
       <c r="L28" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M28" s="6"/>
       <c r="N28" s="6"/>
@@ -3895,27 +3895,27 @@
       <c r="C29" s="24"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H29" s="6" t="str">
         <f t="shared" si="2"/>
         <v>0000010110</v>
       </c>
       <c r="I29" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="J29" s="6" t="s">
         <v>340</v>
       </c>
-      <c r="J29" s="6" t="s">
-        <v>341</v>
-      </c>
       <c r="K29" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="L29" s="6" t="s">
         <v>343</v>
-      </c>
-      <c r="L29" s="6" t="s">
-        <v>344</v>
       </c>
       <c r="M29" s="6"/>
       <c r="N29" s="6"/>
@@ -4073,7 +4073,7 @@
         <v>28</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="6" t="s">
@@ -4113,7 +4113,7 @@
         <v>29</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="6" t="s">
@@ -4210,7 +4210,7 @@
       </c>
       <c r="C39" s="24"/>
       <c r="D39" s="6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
@@ -5117,7 +5117,7 @@
         <v>64</v>
       </c>
       <c r="C71" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>4</v>
@@ -5165,7 +5165,7 @@
         <v>65</v>
       </c>
       <c r="C72" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D72" s="6"/>
       <c r="E72" s="6" t="s">
@@ -5295,7 +5295,7 @@
         <v>69</v>
       </c>
       <c r="C76" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D76" s="22"/>
       <c r="E76" s="22" t="s">
@@ -6104,7 +6104,7 @@
         <v>96</v>
       </c>
       <c r="C103" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D103" s="6" t="s">
         <v>9</v>
@@ -6144,7 +6144,7 @@
         <v>97</v>
       </c>
       <c r="C104" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D104" s="6"/>
       <c r="E104" s="6" t="s">
@@ -6185,7 +6185,7 @@
         <v>98</v>
       </c>
       <c r="C105" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D105" s="6"/>
       <c r="E105" s="6" t="s">
@@ -6223,7 +6223,7 @@
         <v>99</v>
       </c>
       <c r="C106" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D106" s="22"/>
       <c r="E106" s="22" t="s">
@@ -6238,11 +6238,11 @@
         <v>0001100011</v>
       </c>
       <c r="I106" s="22" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="J106" s="22"/>
       <c r="K106" s="22" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L106" s="6"/>
       <c r="M106" s="6"/>
@@ -6261,7 +6261,7 @@
         <v>100</v>
       </c>
       <c r="C107" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D107" s="6"/>
       <c r="E107" s="6" t="s">
@@ -6300,7 +6300,7 @@
         <v>101</v>
       </c>
       <c r="C108" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D108" s="6"/>
       <c r="E108" s="6" t="s">
@@ -6339,7 +6339,7 @@
         <v>102</v>
       </c>
       <c r="C109" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D109" s="6"/>
       <c r="E109" s="6" t="s">
@@ -6377,7 +6377,7 @@
         <v>103</v>
       </c>
       <c r="C110" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D110" s="6"/>
       <c r="E110" s="6" t="s">
@@ -6471,7 +6471,7 @@
         <v>106</v>
       </c>
       <c r="C113" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D113" s="6"/>
       <c r="E113" s="6" t="s">
@@ -6511,7 +6511,7 @@
         <v>107</v>
       </c>
       <c r="C114" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D114" s="6"/>
       <c r="E114" s="6" t="s">
@@ -6551,7 +6551,7 @@
         <v>108</v>
       </c>
       <c r="C115" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D115" s="6"/>
       <c r="E115" s="6" t="s">
@@ -6591,7 +6591,7 @@
         <v>109</v>
       </c>
       <c r="C116" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D116" s="6"/>
       <c r="E116" s="6" t="s">
@@ -6634,7 +6634,7 @@
         <v>110</v>
       </c>
       <c r="C117" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D117" s="6"/>
       <c r="E117" s="6" t="s">
@@ -6674,7 +6674,7 @@
         <v>111</v>
       </c>
       <c r="C118" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D118" s="6"/>
       <c r="E118" s="6" t="s">
@@ -6727,11 +6727,11 @@
         <v>0001110000</v>
       </c>
       <c r="I119" s="22" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="J119" s="22"/>
       <c r="K119" s="22" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="L119" s="10" t="s">
         <v>275</v>
@@ -6765,11 +6765,11 @@
         <v>0001110001</v>
       </c>
       <c r="I120" s="22" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="J120" s="22"/>
       <c r="K120" s="22" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="L120" s="10" t="s">
         <v>275</v>
@@ -6830,7 +6830,7 @@
         <v>115</v>
       </c>
       <c r="C122" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D122" s="6"/>
       <c r="E122" s="6" t="s">
@@ -6851,7 +6851,7 @@
         <v>67</v>
       </c>
       <c r="K122" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="L122" s="10" t="s">
         <v>275</v>
@@ -6931,7 +6931,7 @@
         <v>118</v>
       </c>
       <c r="C125" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D125" s="6"/>
       <c r="E125" s="6" t="s">
@@ -6971,7 +6971,7 @@
         <v>119</v>
       </c>
       <c r="C126" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D126" s="6"/>
       <c r="E126" s="6" t="s">
@@ -7067,7 +7067,7 @@
         <v>122</v>
       </c>
       <c r="C129" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D129" s="6"/>
       <c r="E129" s="6" t="s">
@@ -7250,10 +7250,10 @@
         <v>128</v>
       </c>
       <c r="C135" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D135" s="6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E135" s="6" t="s">
         <v>37</v>
@@ -7279,10 +7279,10 @@
         <v>275</v>
       </c>
       <c r="M135" s="35" t="s">
+        <v>368</v>
+      </c>
+      <c r="N135" s="35" t="s">
         <v>369</v>
-      </c>
-      <c r="N135" s="35" t="s">
-        <v>370</v>
       </c>
       <c r="O135" s="24"/>
       <c r="P135" s="24">
@@ -7302,7 +7302,7 @@
         <v>129</v>
       </c>
       <c r="C136" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D136" s="6"/>
       <c r="E136" s="6" t="s">
@@ -7331,10 +7331,10 @@
         <v>275</v>
       </c>
       <c r="M136" s="35" t="s">
+        <v>368</v>
+      </c>
+      <c r="N136" s="35" t="s">
         <v>369</v>
-      </c>
-      <c r="N136" s="35" t="s">
-        <v>370</v>
       </c>
       <c r="O136" s="24"/>
       <c r="P136" s="24">
@@ -7354,7 +7354,7 @@
         <v>130</v>
       </c>
       <c r="C137" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D137" s="6"/>
       <c r="E137" s="6" t="s">
@@ -7383,10 +7383,10 @@
         <v>275</v>
       </c>
       <c r="M137" s="35" t="s">
+        <v>368</v>
+      </c>
+      <c r="N137" s="35" t="s">
         <v>369</v>
-      </c>
-      <c r="N137" s="35" t="s">
-        <v>370</v>
       </c>
       <c r="O137" s="24"/>
       <c r="P137" s="24">
@@ -7406,7 +7406,7 @@
         <v>131</v>
       </c>
       <c r="C138" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D138" s="6"/>
       <c r="E138" s="6" t="s">
@@ -7452,7 +7452,7 @@
         <v>132</v>
       </c>
       <c r="C139" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D139" s="6"/>
       <c r="E139" s="6" t="s">
@@ -7500,7 +7500,7 @@
         <v>133</v>
       </c>
       <c r="C140" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D140" s="6"/>
       <c r="E140" s="6" t="s">
@@ -7604,14 +7604,14 @@
         <v>136</v>
       </c>
       <c r="C143" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D143" s="6"/>
       <c r="E143" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F143" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G143" s="22" t="s">
         <v>30</v>
@@ -7624,7 +7624,7 @@
         <v>22</v>
       </c>
       <c r="J143" s="22" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="K143" s="6" t="s">
         <v>108</v>
@@ -7696,21 +7696,21 @@
       <c r="C145" s="24"/>
       <c r="D145" s="6"/>
       <c r="E145" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F145" s="6"/>
       <c r="G145" s="22" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H145" s="6" t="str">
         <f t="shared" si="10"/>
         <v>0010001010</v>
       </c>
       <c r="I145" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="J145" s="6" t="s">
         <v>428</v>
-      </c>
-      <c r="J145" s="6" t="s">
-        <v>429</v>
       </c>
       <c r="K145" s="6" t="s">
         <v>176</v>
@@ -7721,13 +7721,13 @@
       <c r="M145" s="6"/>
       <c r="N145" s="6"/>
       <c r="O145" s="24" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="P145" s="24" t="s">
+        <v>430</v>
+      </c>
+      <c r="Q145" s="24" t="s">
         <v>431</v>
-      </c>
-      <c r="Q145" s="24" t="s">
-        <v>432</v>
       </c>
       <c r="R145" s="7"/>
     </row>
@@ -7742,23 +7742,23 @@
       <c r="C146" s="24"/>
       <c r="D146" s="6"/>
       <c r="E146" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F146" s="6" t="s">
         <v>273</v>
       </c>
       <c r="G146" s="22" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H146" s="6" t="str">
         <f t="shared" si="10"/>
         <v>0010001011</v>
       </c>
       <c r="I146" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="J146" s="6" t="s">
         <v>428</v>
-      </c>
-      <c r="J146" s="6" t="s">
-        <v>429</v>
       </c>
       <c r="K146" s="22" t="s">
         <v>177</v>
@@ -7769,13 +7769,13 @@
       <c r="M146" s="6"/>
       <c r="N146" s="6"/>
       <c r="O146" s="24" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="P146" s="24" t="s">
+        <v>430</v>
+      </c>
+      <c r="Q146" s="24" t="s">
         <v>431</v>
-      </c>
-      <c r="Q146" s="24" t="s">
-        <v>432</v>
       </c>
       <c r="R146" s="7"/>
     </row>
@@ -7790,23 +7790,23 @@
       <c r="C147" s="24"/>
       <c r="D147" s="6"/>
       <c r="E147" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F147" s="6" t="s">
         <v>274</v>
       </c>
       <c r="G147" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H147" s="6" t="str">
         <f t="shared" si="10"/>
         <v>0010001100</v>
       </c>
       <c r="I147" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="J147" s="6" t="s">
         <v>428</v>
-      </c>
-      <c r="J147" s="6" t="s">
-        <v>429</v>
       </c>
       <c r="K147" s="22" t="s">
         <v>178</v>
@@ -7817,13 +7817,13 @@
       <c r="M147" s="6"/>
       <c r="N147" s="6"/>
       <c r="O147" s="24" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="P147" s="24" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="Q147" s="24" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="R147" s="7"/>
     </row>
@@ -7838,21 +7838,21 @@
       <c r="C148" s="24"/>
       <c r="D148" s="6"/>
       <c r="E148" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F148" s="6"/>
       <c r="G148" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="H148" s="6" t="str">
         <f t="shared" ref="H148" si="12">DEC2BIN(B148, 10)</f>
         <v>0010001101</v>
       </c>
       <c r="I148" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="J148" s="6" t="s">
         <v>428</v>
-      </c>
-      <c r="J148" s="6" t="s">
-        <v>429</v>
       </c>
       <c r="K148" s="22" t="s">
         <v>170</v>
@@ -7863,13 +7863,13 @@
       <c r="M148" s="6"/>
       <c r="N148" s="6"/>
       <c r="O148" s="24" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="P148" s="24" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="Q148" s="24" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="R148" s="7"/>
     </row>
@@ -7884,23 +7884,23 @@
       <c r="C149" s="24"/>
       <c r="D149" s="6"/>
       <c r="E149" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F149" s="6" t="s">
         <v>273</v>
       </c>
       <c r="G149" s="6" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H149" s="6" t="str">
         <f t="shared" si="10"/>
         <v>0010001110</v>
       </c>
       <c r="I149" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="J149" s="6" t="s">
         <v>428</v>
-      </c>
-      <c r="J149" s="6" t="s">
-        <v>429</v>
       </c>
       <c r="K149" s="22" t="s">
         <v>179</v>
@@ -7911,13 +7911,13 @@
       <c r="M149" s="6"/>
       <c r="N149" s="6"/>
       <c r="O149" s="24" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="P149" s="24" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="Q149" s="24" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="R149" s="7"/>
     </row>
@@ -7932,23 +7932,23 @@
       <c r="C150" s="24"/>
       <c r="D150" s="6"/>
       <c r="E150" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F150" s="6" t="s">
         <v>274</v>
       </c>
       <c r="G150" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="H150" s="6" t="str">
         <f t="shared" si="10"/>
         <v>0010001111</v>
       </c>
       <c r="I150" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="J150" s="6" t="s">
         <v>428</v>
-      </c>
-      <c r="J150" s="6" t="s">
-        <v>429</v>
       </c>
       <c r="K150" s="22" t="s">
         <v>180</v>
@@ -7959,13 +7959,13 @@
       <c r="M150" s="6"/>
       <c r="N150" s="6"/>
       <c r="O150" s="24" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="P150" s="24" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="Q150" s="24" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="R150" s="7"/>
     </row>
@@ -7978,7 +7978,7 @@
         <v>144</v>
       </c>
       <c r="C151" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D151" s="6"/>
       <c r="E151" s="6" t="s">
@@ -8004,7 +8004,7 @@
       </c>
       <c r="M151" s="6"/>
       <c r="N151" s="35" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="O151" s="24"/>
       <c r="P151" s="24">
@@ -8276,34 +8276,34 @@
         <v>154</v>
       </c>
       <c r="C161" s="30" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D161" s="27"/>
       <c r="E161" s="27" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F161" s="27" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G161" s="28" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H161" s="27" t="str">
         <f t="shared" si="10"/>
         <v>0010011010</v>
       </c>
       <c r="I161" s="27" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="J161" s="27"/>
       <c r="K161" s="22" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="L161" s="22" t="s">
         <v>275</v>
       </c>
       <c r="M161" s="22" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="N161" s="22"/>
       <c r="O161" s="30"/>
@@ -8324,34 +8324,34 @@
         <v>155</v>
       </c>
       <c r="C162" s="30" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D162" s="27"/>
       <c r="E162" s="27" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F162" s="27" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G162" s="28" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H162" s="27" t="str">
         <f t="shared" si="10"/>
         <v>0010011011</v>
       </c>
       <c r="I162" s="27" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="J162" s="27"/>
       <c r="K162" s="22" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="L162" s="22" t="s">
         <v>275</v>
       </c>
       <c r="M162" s="22" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="N162" s="22"/>
       <c r="O162" s="30"/>
@@ -8372,34 +8372,34 @@
         <v>156</v>
       </c>
       <c r="C163" s="30" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D163" s="27"/>
       <c r="E163" s="27" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F163" s="27" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G163" s="28" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H163" s="27" t="str">
         <f t="shared" si="10"/>
         <v>0010011100</v>
       </c>
       <c r="I163" s="27" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="J163" s="27"/>
       <c r="K163" s="22" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="L163" s="22" t="s">
         <v>275</v>
       </c>
       <c r="M163" s="22" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="N163" s="22"/>
       <c r="O163" s="30"/>
@@ -8420,28 +8420,28 @@
         <v>157</v>
       </c>
       <c r="C164" s="30" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D164" s="27"/>
       <c r="E164" s="27" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F164" s="27" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G164" s="28" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H164" s="27" t="str">
         <f t="shared" si="10"/>
         <v>0010011101</v>
       </c>
       <c r="I164" s="27" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="J164" s="27"/>
       <c r="K164" s="22" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="L164" s="22" t="s">
         <v>275</v>
@@ -8466,28 +8466,28 @@
         <v>158</v>
       </c>
       <c r="C165" s="30" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D165" s="27"/>
       <c r="E165" s="27" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F165" s="27" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G165" s="28" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="H165" s="27" t="str">
         <f t="shared" si="10"/>
         <v>0010011110</v>
       </c>
       <c r="I165" s="27" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="J165" s="27"/>
       <c r="K165" s="22" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="L165" s="22" t="s">
         <v>275</v>
@@ -8512,28 +8512,28 @@
         <v>159</v>
       </c>
       <c r="C166" s="30" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D166" s="27"/>
       <c r="E166" s="27" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F166" s="27" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G166" s="28" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H166" s="27" t="str">
         <f t="shared" si="10"/>
         <v>0010011111</v>
       </c>
       <c r="I166" s="27" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="J166" s="27"/>
       <c r="K166" s="22" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="L166" s="22" t="s">
         <v>275</v>
@@ -8558,7 +8558,7 @@
         <v>160</v>
       </c>
       <c r="C167" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D167" s="6" t="s">
         <v>48</v>
@@ -8610,7 +8610,7 @@
         <v>161</v>
       </c>
       <c r="C168" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D168" s="6"/>
       <c r="E168" s="6" t="s">
@@ -8660,7 +8660,7 @@
         <v>162</v>
       </c>
       <c r="C169" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D169" s="6"/>
       <c r="E169" s="6" t="s">
@@ -8710,7 +8710,7 @@
         <v>163</v>
       </c>
       <c r="C170" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D170" s="6"/>
       <c r="E170" s="6" t="s">
@@ -9602,7 +9602,7 @@
         <v>192</v>
       </c>
       <c r="C199" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D199" s="6" t="s">
         <v>69</v>
@@ -9796,7 +9796,7 @@
         <v>197</v>
       </c>
       <c r="C204" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D204" s="6"/>
       <c r="E204" s="22" t="s">
@@ -9919,7 +9919,7 @@
       <c r="M207" s="6"/>
       <c r="N207" s="10"/>
       <c r="O207" s="24" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="P207" s="24">
         <v>3</v>
@@ -9963,7 +9963,7 @@
       <c r="M208" s="6"/>
       <c r="N208" s="6"/>
       <c r="O208" s="24" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="P208" s="24">
         <v>3</v>
@@ -10098,7 +10098,7 @@
         <v>205</v>
       </c>
       <c r="C212" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D212" s="6"/>
       <c r="E212" s="34" t="s">
@@ -10136,7 +10136,7 @@
         <v>206</v>
       </c>
       <c r="C213" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D213" s="6"/>
       <c r="E213" s="6" t="s">
@@ -10304,7 +10304,7 @@
         <v>211</v>
       </c>
       <c r="C218" s="24" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D218" s="22"/>
       <c r="E218" s="22" t="s">
@@ -10342,27 +10342,27 @@
         <v>212</v>
       </c>
       <c r="C219" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D219" s="22"/>
       <c r="E219" s="22" t="s">
-        <v>304</v>
+        <v>437</v>
       </c>
       <c r="F219" s="22"/>
       <c r="G219" s="22" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H219" s="22" t="str">
         <f t="shared" si="17"/>
         <v>0011010100</v>
       </c>
       <c r="I219" s="22" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="J219" s="22"/>
       <c r="K219" s="22"/>
       <c r="L219" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="M219" s="22"/>
       <c r="N219" s="6"/>
@@ -10379,26 +10379,28 @@
       <c r="B220" s="22">
         <v>213</v>
       </c>
-      <c r="C220" s="24"/>
+      <c r="C220" s="24" t="s">
+        <v>435</v>
+      </c>
       <c r="D220" s="22"/>
       <c r="E220" s="22" t="s">
         <v>303</v>
       </c>
       <c r="F220" s="22"/>
       <c r="G220" s="22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H220" s="22" t="str">
         <f t="shared" si="17"/>
         <v>0011010101</v>
       </c>
       <c r="I220" s="22" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J220" s="22"/>
       <c r="K220" s="22"/>
       <c r="L220" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="M220" s="22"/>
       <c r="N220" s="6"/>
@@ -10415,26 +10417,28 @@
       <c r="B221" s="22">
         <v>214</v>
       </c>
-      <c r="C221" s="24"/>
+      <c r="C221" s="24" t="s">
+        <v>435</v>
+      </c>
       <c r="D221" s="22"/>
       <c r="E221" s="22" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F221" s="22"/>
       <c r="G221" s="22" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H221" s="22" t="str">
         <f t="shared" si="17"/>
         <v>0011010110</v>
       </c>
       <c r="I221" s="22" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J221" s="22"/>
       <c r="K221" s="22"/>
       <c r="L221" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="M221" s="22"/>
       <c r="N221" s="6"/>
@@ -10452,29 +10456,29 @@
         <v>215</v>
       </c>
       <c r="C222" s="24" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D222" s="32"/>
       <c r="E222" s="32" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F222" s="32"/>
       <c r="G222" s="32" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H222" s="32" t="str">
         <f t="shared" si="17"/>
         <v>0011010111</v>
       </c>
       <c r="I222" s="32" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="J222" s="32"/>
       <c r="K222" s="32" t="s">
+        <v>328</v>
+      </c>
+      <c r="L222" s="32" t="s">
         <v>329</v>
-      </c>
-      <c r="L222" s="32" t="s">
-        <v>330</v>
       </c>
       <c r="M222" s="32"/>
       <c r="N222" s="6"/>
@@ -10492,29 +10496,29 @@
         <v>216</v>
       </c>
       <c r="C223" s="24" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D223" s="6"/>
       <c r="E223" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F223" s="6"/>
       <c r="G223" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H223" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011011000</v>
       </c>
       <c r="I223" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="J223" s="6"/>
       <c r="K223" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="L223" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="M223" s="6"/>
       <c r="N223" s="6"/>
@@ -10532,29 +10536,29 @@
         <v>217</v>
       </c>
       <c r="C224" s="24" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D224" s="6"/>
       <c r="E224" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F224" s="6"/>
       <c r="G224" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H224" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011011001</v>
       </c>
       <c r="I224" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="J224" s="6"/>
       <c r="K224" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="L224" s="6" t="s">
         <v>409</v>
-      </c>
-      <c r="L224" s="6" t="s">
-        <v>410</v>
       </c>
       <c r="M224" s="6"/>
       <c r="N224" s="6"/>
@@ -10740,7 +10744,7 @@
         <v>224</v>
       </c>
       <c r="C231" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D231" s="6" t="s">
         <v>70</v>
@@ -10750,7 +10754,7 @@
       </c>
       <c r="F231" s="6"/>
       <c r="G231" s="22" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H231" s="6" t="str">
         <f t="shared" si="17"/>
@@ -10784,11 +10788,11 @@
       <c r="C232" s="24"/>
       <c r="D232" s="32"/>
       <c r="E232" s="32" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F232" s="32"/>
       <c r="G232" s="32" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H232" s="32" t="str">
         <f t="shared" si="17"/>
@@ -10805,7 +10809,7 @@
       <c r="M232" s="32"/>
       <c r="N232" s="6"/>
       <c r="O232" s="24" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="P232" s="24"/>
       <c r="Q232" s="24" t="s">
@@ -10908,7 +10912,7 @@
         <v>229</v>
       </c>
       <c r="C236" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D236" s="6"/>
       <c r="E236" s="22" t="s">
@@ -11206,7 +11210,7 @@
         <v>237</v>
       </c>
       <c r="C244" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D244" s="6"/>
       <c r="E244" s="34" t="s">
@@ -11244,7 +11248,7 @@
         <v>238</v>
       </c>
       <c r="C245" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D245" s="6"/>
       <c r="E245" s="6" t="s">
@@ -11384,7 +11388,7 @@
         <v>242</v>
       </c>
       <c r="C249" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D249" s="22"/>
       <c r="E249" s="22" t="s">
@@ -11422,7 +11426,7 @@
         <v>243</v>
       </c>
       <c r="C250" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D250" s="22"/>
       <c r="E250" s="22" t="s">
@@ -11460,27 +11464,27 @@
         <v>244</v>
       </c>
       <c r="C251" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D251" s="22"/>
       <c r="E251" s="22" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F251" s="22"/>
       <c r="G251" s="22" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H251" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011110100</v>
       </c>
       <c r="I251" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="J251" s="6"/>
       <c r="K251" s="6"/>
       <c r="L251" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="M251" s="22"/>
       <c r="N251" s="6"/>
@@ -11498,27 +11502,27 @@
         <v>245</v>
       </c>
       <c r="C252" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D252" s="22"/>
       <c r="E252" s="22" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F252" s="22"/>
       <c r="G252" s="22" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H252" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011110101</v>
       </c>
       <c r="I252" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J252" s="6"/>
       <c r="K252" s="6"/>
       <c r="L252" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="M252" s="22"/>
       <c r="N252" s="6"/>
@@ -11536,27 +11540,27 @@
         <v>246</v>
       </c>
       <c r="C253" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D253" s="22"/>
       <c r="E253" s="22" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F253" s="22"/>
       <c r="G253" s="22" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H253" s="6" t="str">
         <f t="shared" si="17"/>
         <v>0011110110</v>
       </c>
       <c r="I253" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J253" s="6"/>
       <c r="K253" s="6"/>
       <c r="L253" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="M253" s="22"/>
       <c r="N253" s="6"/>
@@ -11798,17 +11802,17 @@
         <v>255</v>
       </c>
       <c r="C262" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D262" s="35"/>
       <c r="E262" s="35" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F262" s="35" t="s">
         <v>277</v>
       </c>
       <c r="G262" s="35" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H262" s="35" t="str">
         <f t="shared" si="17"/>
@@ -11816,10 +11820,10 @@
       </c>
       <c r="I262" s="35"/>
       <c r="J262" s="35" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="K262" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="L262" s="6" t="s">
         <v>275</v>
@@ -11840,7 +11844,7 @@
         <v>256</v>
       </c>
       <c r="C263" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D263" s="6" t="s">
         <v>25</v>
@@ -11907,7 +11911,7 @@
       <c r="M264" s="6"/>
       <c r="N264" s="6"/>
       <c r="O264" s="24" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="P264" s="24">
         <v>3</v>
@@ -11926,7 +11930,7 @@
         <v>258</v>
       </c>
       <c r="C265" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D265" s="6"/>
       <c r="E265" s="6" t="s">
@@ -11966,7 +11970,7 @@
         <v>259</v>
       </c>
       <c r="C266" s="24" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D266" s="6"/>
       <c r="E266" s="6" t="s">
@@ -12794,7 +12798,7 @@
         <v>288</v>
       </c>
       <c r="C295" s="24" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D295" s="6" t="s">
         <v>283</v>
@@ -12849,13 +12853,13 @@
         <v>0100100001</v>
       </c>
       <c r="I296" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="J296" s="6" t="s">
         <v>391</v>
       </c>
-      <c r="J296" s="6" t="s">
+      <c r="K296" s="6" t="s">
         <v>392</v>
-      </c>
-      <c r="K296" s="6" t="s">
-        <v>393</v>
       </c>
       <c r="L296" s="35" t="s">
         <v>275</v>
@@ -12875,7 +12879,9 @@
       <c r="B297" s="6">
         <v>290</v>
       </c>
-      <c r="C297" s="39"/>
+      <c r="C297" s="24" t="s">
+        <v>434</v>
+      </c>
       <c r="D297" s="6"/>
       <c r="E297" s="27" t="s">
         <v>290</v>
@@ -12923,11 +12929,11 @@
       <c r="C298" s="24"/>
       <c r="D298" s="6"/>
       <c r="E298" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F298" s="6"/>
       <c r="G298" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H298" s="6" t="str">
         <f t="shared" si="20"/>
@@ -12955,11 +12961,11 @@
       <c r="C299" s="24"/>
       <c r="D299" s="6"/>
       <c r="E299" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F299" s="6"/>
       <c r="G299" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H299" s="6" t="str">
         <f t="shared" si="20"/>

</xml_diff>

<commit_message>
added instruction(type-e) : rev8
</commit_message>
<xml_diff>
--- a/instructions/mist32_isa.xlsx
+++ b/instructions/mist32_isa.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="7020" yWindow="1500" windowWidth="16110" windowHeight="7815"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="438">
   <si>
     <t>ADD</t>
     <phoneticPr fontId="1"/>
@@ -2910,8 +2910,8 @@
   </sheetPr>
   <dimension ref="A2:AL1031"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A281" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C295" sqref="C295"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C120" sqref="C120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6751,7 +6751,9 @@
       <c r="B120" s="22">
         <v>113</v>
       </c>
-      <c r="C120" s="24"/>
+      <c r="C120" s="24" t="s">
+        <v>435</v>
+      </c>
       <c r="D120" s="22"/>
       <c r="E120" s="22" t="s">
         <v>77</v>

</xml_diff>